<commit_message>
Dates now format to regional settings
</commit_message>
<xml_diff>
--- a/Lava3.Test/TestFiles/Test.xlsx
+++ b/Lava3.Test/TestFiles/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="585" windowWidth="15555" windowHeight="18030" tabRatio="554" activeTab="3"/>
+    <workbookView xWindow="510" yWindow="585" windowWidth="15555" windowHeight="18030" tabRatio="554" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Annual Summary" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
   <si>
     <t>Description</t>
   </si>
@@ -165,15 +165,9 @@
     <t xml:space="preserve">COMPANIES HOUSE        CARDIFF       GB </t>
   </si>
   <si>
-    <t xml:space="preserve">ADOBE  PHOTOGPHY PLAN  800 833 6687  IE </t>
-  </si>
-  <si>
     <t xml:space="preserve">DISCLOSURE SCOT        EDINBURGH     GB </t>
   </si>
   <si>
-    <t xml:space="preserve">IPSE                   0208 8979970  GB </t>
-  </si>
-  <si>
     <t>BANK ACCOUNT PAYMENTS</t>
   </si>
   <si>
@@ -324,9 +318,6 @@
     <t>ACME Consulting</t>
   </si>
   <si>
-    <t>Apple Food</t>
-  </si>
-  <si>
     <t>Bugs Bunny Mobile</t>
   </si>
   <si>
@@ -346,6 +337,12 @@
   </si>
   <si>
     <t>ACME - Salary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADOBE  PHOTOGPHY PLAN  8087  IE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPSE                   0970  GB </t>
   </si>
 </sst>
 </file>
@@ -365,10 +362,17 @@
     <numFmt numFmtId="171" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="46">
+  <fonts count="47">
     <font>
       <sz val="10"/>
       <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1045,952 +1049,952 @@
   </borders>
   <cellStyleXfs count="931">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="22" borderId="9"/>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="12"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="35" fillId="19" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="6"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="7"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="8"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="37" fillId="21" borderId="9"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="11"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="22" borderId="9"/>
+    <xf numFmtId="0" fontId="42" fillId="23" borderId="12"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="19" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="6"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="7"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="8"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="9"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="11"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="38" fillId="22" borderId="10"/>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="13"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="22" borderId="10"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="13"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="147">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1998,151 +2002,151 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="25" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="26" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="748" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="748" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="17" fillId="18" borderId="1" xfId="748" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="17" fillId="18" borderId="1" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="18" fillId="18" borderId="1" xfId="748" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="18" fillId="18" borderId="1" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="18" fillId="0" borderId="1" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="927" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="19" fillId="0" borderId="1" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="927" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="802" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="802" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="2" borderId="3" xfId="850" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="2" borderId="3" xfId="850" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="29" fillId="2" borderId="4" xfId="850" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="30" fillId="2" borderId="4" xfId="850" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="29" fillId="2" borderId="0" xfId="850" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="30" fillId="2" borderId="0" xfId="850" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="26" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="27" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="27" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="770" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="770" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="24" fillId="12" borderId="5" xfId="743" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="25" fillId="12" borderId="5" xfId="743" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="770" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="25" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="770" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="26" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="748" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="763" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" xfId="763" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="44" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="44" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="44" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2156,64 +2160,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="17" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="18" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="923" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" xfId="800" applyFont="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="3" fillId="35" borderId="0" xfId="800" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="3" fillId="2" borderId="2" xfId="923" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="770"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="923" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" xfId="800" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="2" fillId="35" borderId="0" xfId="800" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="2" xfId="923" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="923" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="763" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="44" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="44" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="44" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="44" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="770"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="923" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" xfId="763" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="931">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -3535,7 +3539,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="12.75">
       <c r="A1" s="87" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B1" s="87"/>
       <c r="D1" s="23"/>
@@ -3563,7 +3567,7 @@
     </row>
     <row r="2" spans="1:25" ht="12.75">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3"/>
       <c r="D2" s="23"/>
@@ -3591,13 +3595,13 @@
     </row>
     <row r="3" spans="1:25" ht="12.75">
       <c r="E3" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="135" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
+        <v>49</v>
+      </c>
+      <c r="F3" s="137" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="25"/>
@@ -3616,21 +3620,21 @@
       <c r="X3" s="24"/>
       <c r="Y3" s="24"/>
     </row>
-    <row r="4" spans="1:25" s="114" customFormat="1" ht="12.75">
+    <row r="4" spans="1:25" s="113" customFormat="1" ht="12.75">
       <c r="A4" s="66" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="E4" s="36" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>56</v>
       </c>
       <c r="F4" s="36" t="s">
         <v>8</v>
@@ -3660,16 +3664,16 @@
       <c r="W4" s="24"/>
       <c r="X4" s="24"/>
     </row>
-    <row r="5" spans="1:25" s="115" customFormat="1" ht="12.75">
-      <c r="A5" s="118"/>
+    <row r="5" spans="1:25" s="114" customFormat="1" ht="12.75">
+      <c r="A5" s="117"/>
       <c r="B5" s="64"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
-      <c r="I5" s="117"/>
+      <c r="I5" s="116"/>
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
       <c r="L5" s="27"/>
@@ -3686,37 +3690,37 @@
       <c r="W5" s="24"/>
       <c r="X5" s="24"/>
     </row>
-    <row r="6" spans="1:25" s="115" customFormat="1" ht="12.75">
+    <row r="6" spans="1:25" s="114" customFormat="1" ht="12.75">
       <c r="A6" s="68"/>
       <c r="B6" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="120">
-        <f>SUM(C5:C5)</f>
+        <v>55</v>
+      </c>
+      <c r="C6" s="119">
+        <f t="shared" ref="C6:I6" si="0">SUM(C5:C5)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="120">
-        <f>SUM(D5:D5)</f>
+      <c r="D6" s="119">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="120">
-        <f>SUM(E5:E5)</f>
+      <c r="E6" s="119">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="120">
-        <f>SUM(F5:F5)</f>
+      <c r="F6" s="119">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="120">
-        <f>SUM(G5:G5)</f>
+      <c r="G6" s="119">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="120">
-        <f>SUM(H5:H5)</f>
+      <c r="H6" s="119">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="120">
-        <f>SUM(I5:I5)</f>
+      <c r="I6" s="119">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J6" s="27"/>
@@ -3735,16 +3739,16 @@
       <c r="W6" s="24"/>
       <c r="X6" s="24"/>
     </row>
-    <row r="7" spans="1:25" s="115" customFormat="1" ht="12.75">
+    <row r="7" spans="1:25" s="114" customFormat="1" ht="12.75">
       <c r="A7" s="110"/>
       <c r="B7" s="64"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
-      <c r="I7" s="117"/>
+      <c r="I7" s="116"/>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
       <c r="L7" s="27"/>
@@ -3839,10 +3843,10 @@
       <c r="X10" s="24"/>
     </row>
     <row r="11" spans="1:25" ht="12.75">
-      <c r="A11" s="132" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="132"/>
+      <c r="A11" s="134" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="134"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
@@ -3867,11 +3871,11 @@
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1">
       <c r="C12" s="23"/>
-      <c r="D12" s="133" t="s">
-        <v>59</v>
+      <c r="D12" s="135" t="s">
+        <v>57</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="34"/>
@@ -3892,11 +3896,11 @@
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="134"/>
+        <v>58</v>
+      </c>
+      <c r="D13" s="136"/>
       <c r="E13" s="34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>11</v>
@@ -4067,15 +4071,15 @@
         <v>0</v>
       </c>
       <c r="E20" s="19">
-        <f t="shared" ref="E20:G20" si="0">SUM(E14:E19)</f>
+        <f t="shared" ref="E20:G20" si="1">SUM(E14:E19)</f>
         <v>0</v>
       </c>
       <c r="F20" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G20" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H20" s="19">
@@ -4126,11 +4130,11 @@
       <c r="X21" s="24"/>
     </row>
     <row r="22" spans="1:28" ht="12.75">
-      <c r="A22" s="132" t="str">
+      <c r="A22" s="134" t="str">
         <f>A1</f>
         <v>ACME Consulting</v>
       </c>
-      <c r="B22" s="132"/>
+      <c r="B22" s="134"/>
       <c r="C22" s="3"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
@@ -4154,7 +4158,7 @@
     </row>
     <row r="23" spans="1:28" ht="12.75" customHeight="1">
       <c r="A23" s="46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F23" s="79"/>
       <c r="I23" s="3"/>
@@ -4177,28 +4181,28 @@
     <row r="24" spans="1:28" ht="12.75" customHeight="1">
       <c r="A24" s="4"/>
       <c r="B24" s="95" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="96" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="96" t="s">
+      <c r="E24" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="96" t="s">
+      <c r="F24" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="96" t="s">
+      <c r="G24" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="80" t="s">
+      <c r="H24" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="96" t="s">
+      <c r="I24" s="47" t="s">
         <v>68</v>
-      </c>
-      <c r="H24" s="96" t="s">
-        <v>69</v>
-      </c>
-      <c r="I24" s="47" t="s">
-        <v>70</v>
       </c>
       <c r="N24" s="12"/>
       <c r="O24" s="26"/>
@@ -4221,7 +4225,7 @@
       <c r="B25" s="93"/>
       <c r="C25" s="92"/>
       <c r="D25" s="83"/>
-      <c r="E25" s="116"/>
+      <c r="E25" s="115"/>
       <c r="F25" s="97"/>
       <c r="G25" s="14"/>
       <c r="H25" s="15"/>
@@ -4244,7 +4248,7 @@
       <c r="AA25" s="24"/>
       <c r="AB25" s="24"/>
     </row>
-    <row r="26" spans="1:28" s="114" customFormat="1" ht="15.75">
+    <row r="26" spans="1:28" s="113" customFormat="1" ht="15.75">
       <c r="A26" s="111"/>
       <c r="B26" s="93"/>
       <c r="C26" s="11"/>
@@ -4303,7 +4307,7 @@
     <row r="28" spans="1:28" ht="12.75">
       <c r="A28" s="30"/>
       <c r="B28" s="36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
@@ -4344,7 +4348,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="81" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J29" s="24"/>
       <c r="K29" s="24"/>
@@ -4784,12 +4788,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet2" filterMode="1"/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -4813,10 +4817,10 @@
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
       <c r="E1" s="44"/>
-      <c r="F1" s="136" t="s">
+      <c r="F1" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="136"/>
+      <c r="G1" s="138"/>
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
     </row>
@@ -4849,145 +4853,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="129" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="130">
+    <row r="3" spans="1:9" s="128" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="129">
         <v>42466</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="129">
+      <c r="G3" s="128">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="129" customFormat="1" ht="15">
-      <c r="A4" s="130">
+    <row r="4" spans="1:9" s="128" customFormat="1" ht="15">
+      <c r="A4" s="129">
         <v>42468</v>
       </c>
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="128" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="129">
+      <c r="C4" s="128">
         <v>23.62</v>
       </c>
-      <c r="D4" s="129">
+      <c r="D4" s="128">
         <v>0</v>
       </c>
-      <c r="E4" s="129">
+      <c r="E4" s="128">
         <v>76.38</v>
       </c>
-      <c r="F4" s="129">
+      <c r="F4" s="128">
         <v>-23.62</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="129" customFormat="1" ht="15">
-      <c r="A5" s="130">
+    <row r="5" spans="1:9" s="128" customFormat="1" ht="15">
+      <c r="A5" s="129">
         <v>42471</v>
       </c>
-      <c r="B5" s="129" t="s">
+      <c r="B5" s="128" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="129">
+      <c r="C5" s="128">
         <v>0.96</v>
       </c>
-      <c r="D5" s="129">
+      <c r="D5" s="128">
         <v>0</v>
       </c>
-      <c r="E5" s="129">
+      <c r="E5" s="128">
         <v>75.42</v>
       </c>
-      <c r="F5" s="129">
+      <c r="F5" s="128">
         <v>-24.580000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="128" customFormat="1" ht="15">
-      <c r="A6" s="131">
+    <row r="6" spans="1:9" s="127" customFormat="1" ht="15">
+      <c r="A6" s="130">
         <v>42609</v>
       </c>
-      <c r="B6" s="146" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="128">
+      <c r="B6" s="133" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="127">
         <v>3.1</v>
       </c>
-      <c r="D6" s="128">
+      <c r="D6" s="127">
         <v>0</v>
       </c>
-      <c r="E6" s="128">
+      <c r="E6" s="127">
         <v>72.320000000000007</v>
       </c>
-      <c r="F6" s="128">
+      <c r="F6" s="127">
         <v>-3.1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="128" customFormat="1" ht="15">
-      <c r="A7" s="131">
+    <row r="7" spans="1:9" s="127" customFormat="1" ht="15">
+      <c r="A7" s="130">
         <v>42610</v>
       </c>
-      <c r="B7" s="128" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="128">
+      <c r="B7" s="127" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="127">
         <v>0</v>
       </c>
-      <c r="D7" s="128">
+      <c r="D7" s="127">
         <v>1000</v>
       </c>
-      <c r="E7" s="128">
+      <c r="E7" s="127">
         <v>1072.32</v>
       </c>
-      <c r="F7" s="128">
+      <c r="F7" s="127">
         <v>996.9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="128" customFormat="1" ht="15">
-      <c r="A8" s="131">
+    <row r="8" spans="1:9" s="127" customFormat="1" ht="15">
+      <c r="A8" s="130">
         <v>42611</v>
       </c>
-      <c r="B8" s="128" t="s">
+      <c r="B8" s="127" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="128">
+      <c r="C8" s="127">
         <v>34.99</v>
       </c>
-      <c r="D8" s="128">
+      <c r="D8" s="127">
         <v>0</v>
       </c>
-      <c r="E8" s="128">
+      <c r="E8" s="127">
         <v>1037.33</v>
       </c>
-      <c r="F8" s="128">
+      <c r="F8" s="127">
         <v>961.91</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="128" customFormat="1" ht="15">
-      <c r="A9" s="131">
+    <row r="9" spans="1:9" s="127" customFormat="1" ht="15">
+      <c r="A9" s="130">
         <v>42612</v>
       </c>
-      <c r="B9" s="146" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="128">
+      <c r="B9" s="132" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="127">
         <v>14.5</v>
       </c>
-      <c r="D9" s="128">
+      <c r="D9" s="127">
         <v>0</v>
       </c>
-      <c r="E9" s="128">
+      <c r="E9" s="127">
         <v>1022.8299999999999</v>
       </c>
-      <c r="F9" s="128">
+      <c r="F9" s="127">
         <v>947.41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I5">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="EUROBASE SYS LTD"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState ref="A3:I43">
     <sortCondition ref="A3:A43"/>
     <sortCondition ref="E3:E43"/>
@@ -5007,7 +5004,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -5056,22 +5053,22 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="74" customFormat="1" ht="15">
-      <c r="A2" s="118">
+      <c r="A2" s="117">
         <v>42611</v>
       </c>
       <c r="B2" s="39">
         <v>42592</v>
       </c>
-      <c r="C2" s="118">
+      <c r="C2" s="117">
         <v>42524</v>
       </c>
       <c r="D2" s="112" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="121">
+      <c r="E2" s="120">
         <v>-10</v>
       </c>
-      <c r="F2" s="123"/>
+      <c r="F2" s="122"/>
       <c r="G2" s="74">
         <v>3</v>
       </c>
@@ -5082,7 +5079,7 @@
       <c r="J2" s="72"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="118">
+      <c r="A3" s="117">
         <v>42611</v>
       </c>
       <c r="B3" s="39">
@@ -5097,12 +5094,12 @@
       <c r="E3" s="61">
         <v>-13</v>
       </c>
-      <c r="F3" s="123"/>
+      <c r="F3" s="122"/>
       <c r="I3" s="74"/>
       <c r="J3" s="74"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="118">
+      <c r="A4" s="117">
         <v>42611</v>
       </c>
       <c r="B4" s="39">
@@ -5111,13 +5108,13 @@
       <c r="C4" s="104">
         <v>42562</v>
       </c>
-      <c r="D4" s="126" t="s">
+      <c r="D4" s="125" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="61">
         <v>-11.99</v>
       </c>
-      <c r="F4" s="123"/>
+      <c r="F4" s="122"/>
       <c r="I4" s="74"/>
       <c r="J4" s="74"/>
     </row>
@@ -5127,13 +5124,13 @@
       <c r="C5" s="111">
         <v>42581</v>
       </c>
-      <c r="D5" s="127" t="s">
-        <v>102</v>
+      <c r="D5" s="126" t="s">
+        <v>99</v>
       </c>
       <c r="E5" s="61">
         <v>-22.15</v>
       </c>
-      <c r="F5" s="123"/>
+      <c r="F5" s="122"/>
       <c r="G5" s="75">
         <v>4</v>
       </c>
@@ -5149,13 +5146,13 @@
       <c r="C6" s="111">
         <v>42581</v>
       </c>
-      <c r="D6" s="127" t="s">
-        <v>92</v>
+      <c r="D6" s="126" t="s">
+        <v>90</v>
       </c>
       <c r="E6" s="61">
         <v>-0.66</v>
       </c>
-      <c r="F6" s="123"/>
+      <c r="F6" s="122"/>
       <c r="G6" s="75"/>
       <c r="H6" s="75"/>
       <c r="I6" s="73"/>
@@ -5167,13 +5164,13 @@
       <c r="C7" s="111">
         <v>42585</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>47</v>
+      <c r="D7" s="126" t="s">
+        <v>105</v>
       </c>
       <c r="E7" s="61">
         <v>-6.85</v>
       </c>
-      <c r="F7" s="123"/>
+      <c r="F7" s="122"/>
       <c r="G7" s="75"/>
       <c r="H7" s="75"/>
       <c r="I7" s="73"/>
@@ -5185,51 +5182,51 @@
         <v>42590</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="61">
         <v>-25</v>
       </c>
-      <c r="F8" s="123"/>
+      <c r="F8" s="122"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="39"/>
       <c r="C9" s="111">
         <v>42592</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>49</v>
+      <c r="D9" s="126" t="s">
+        <v>106</v>
       </c>
       <c r="E9" s="61">
         <v>-174</v>
       </c>
-      <c r="F9" s="123"/>
+      <c r="F9" s="122"/>
     </row>
     <row r="10" spans="1:10">
       <c r="B10" s="39"/>
       <c r="C10" s="111">
         <v>42593</v>
       </c>
-      <c r="D10" s="127" t="s">
-        <v>103</v>
+      <c r="D10" s="126" t="s">
+        <v>100</v>
       </c>
       <c r="E10" s="61">
         <v>-35.020000000000003</v>
       </c>
-      <c r="F10" s="123"/>
+      <c r="F10" s="122"/>
     </row>
     <row r="11" spans="1:10">
       <c r="B11" s="39"/>
       <c r="C11" s="111">
         <v>42594</v>
       </c>
-      <c r="D11" s="127" t="s">
-        <v>103</v>
+      <c r="D11" s="126" t="s">
+        <v>100</v>
       </c>
       <c r="E11" s="61">
         <v>-11.99</v>
       </c>
-      <c r="F11" s="123"/>
+      <c r="F11" s="122"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="111"/>
@@ -5237,10 +5234,10 @@
       <c r="C12" s="111"/>
       <c r="D12" s="8"/>
       <c r="E12" s="61"/>
-      <c r="F12" s="123"/>
+      <c r="F12" s="122"/>
       <c r="G12" s="75"/>
       <c r="I12" s="73"/>
-      <c r="J12" s="114"/>
+      <c r="J12" s="113"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="111"/>
@@ -5248,165 +5245,165 @@
       <c r="C13" s="111"/>
       <c r="D13" s="8"/>
       <c r="E13" s="61"/>
-      <c r="F13" s="123"/>
+      <c r="F13" s="122"/>
       <c r="I13" s="73"/>
     </row>
     <row r="14" spans="1:10">
       <c r="B14" s="39"/>
       <c r="C14" s="74"/>
       <c r="D14" s="74"/>
-      <c r="E14" s="122"/>
-      <c r="F14" s="123"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="122"/>
     </row>
     <row r="15" spans="1:10">
       <c r="B15" s="39"/>
-      <c r="E15" s="122"/>
-      <c r="F15" s="123"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="122"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="E16" s="122"/>
-      <c r="F16" s="123"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="122"/>
     </row>
     <row r="17" spans="5:6">
-      <c r="E17" s="122"/>
-      <c r="F17" s="123"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="122"/>
     </row>
     <row r="18" spans="5:6">
-      <c r="E18" s="122"/>
-      <c r="F18" s="123"/>
+      <c r="E18" s="121"/>
+      <c r="F18" s="122"/>
     </row>
     <row r="19" spans="5:6">
-      <c r="E19" s="122"/>
-      <c r="F19" s="123"/>
+      <c r="E19" s="121"/>
+      <c r="F19" s="122"/>
     </row>
     <row r="20" spans="5:6">
-      <c r="E20" s="122"/>
-      <c r="F20" s="123"/>
+      <c r="E20" s="121"/>
+      <c r="F20" s="122"/>
     </row>
     <row r="21" spans="5:6">
-      <c r="E21" s="122"/>
-      <c r="F21" s="123"/>
+      <c r="E21" s="121"/>
+      <c r="F21" s="122"/>
     </row>
     <row r="22" spans="5:6">
-      <c r="E22" s="122"/>
-      <c r="F22" s="123"/>
+      <c r="E22" s="121"/>
+      <c r="F22" s="122"/>
     </row>
     <row r="23" spans="5:6">
-      <c r="E23" s="122"/>
+      <c r="E23" s="121"/>
     </row>
     <row r="24" spans="5:6">
-      <c r="E24" s="122"/>
+      <c r="E24" s="121"/>
     </row>
     <row r="25" spans="5:6">
-      <c r="E25" s="122"/>
+      <c r="E25" s="121"/>
     </row>
     <row r="26" spans="5:6">
-      <c r="E26" s="122"/>
+      <c r="E26" s="121"/>
     </row>
     <row r="27" spans="5:6">
-      <c r="E27" s="122"/>
+      <c r="E27" s="121"/>
     </row>
     <row r="28" spans="5:6">
-      <c r="E28" s="122"/>
+      <c r="E28" s="121"/>
     </row>
     <row r="29" spans="5:6">
-      <c r="E29" s="122"/>
+      <c r="E29" s="121"/>
     </row>
     <row r="30" spans="5:6">
-      <c r="E30" s="122"/>
+      <c r="E30" s="121"/>
     </row>
     <row r="31" spans="5:6">
-      <c r="E31" s="122"/>
+      <c r="E31" s="121"/>
     </row>
     <row r="32" spans="5:6">
-      <c r="E32" s="122"/>
+      <c r="E32" s="121"/>
     </row>
     <row r="33" spans="5:5">
-      <c r="E33" s="122"/>
+      <c r="E33" s="121"/>
     </row>
     <row r="34" spans="5:5">
-      <c r="E34" s="122"/>
+      <c r="E34" s="121"/>
     </row>
     <row r="35" spans="5:5">
-      <c r="E35" s="122"/>
+      <c r="E35" s="121"/>
     </row>
     <row r="36" spans="5:5">
-      <c r="E36" s="122"/>
+      <c r="E36" s="121"/>
     </row>
     <row r="37" spans="5:5">
-      <c r="E37" s="122"/>
+      <c r="E37" s="121"/>
     </row>
     <row r="38" spans="5:5">
-      <c r="E38" s="122"/>
+      <c r="E38" s="121"/>
     </row>
     <row r="39" spans="5:5">
-      <c r="E39" s="122"/>
+      <c r="E39" s="121"/>
     </row>
     <row r="40" spans="5:5">
-      <c r="E40" s="122"/>
+      <c r="E40" s="121"/>
     </row>
     <row r="41" spans="5:5">
-      <c r="E41" s="122"/>
+      <c r="E41" s="121"/>
     </row>
     <row r="42" spans="5:5">
-      <c r="E42" s="122"/>
+      <c r="E42" s="121"/>
     </row>
     <row r="43" spans="5:5">
-      <c r="E43" s="122"/>
+      <c r="E43" s="121"/>
     </row>
     <row r="44" spans="5:5">
-      <c r="E44" s="122"/>
+      <c r="E44" s="121"/>
     </row>
     <row r="45" spans="5:5">
-      <c r="E45" s="122"/>
+      <c r="E45" s="121"/>
     </row>
     <row r="46" spans="5:5">
-      <c r="E46" s="122"/>
+      <c r="E46" s="121"/>
     </row>
     <row r="47" spans="5:5">
-      <c r="E47" s="122"/>
+      <c r="E47" s="121"/>
     </row>
     <row r="48" spans="5:5">
-      <c r="E48" s="122"/>
+      <c r="E48" s="121"/>
     </row>
     <row r="49" spans="5:5">
-      <c r="E49" s="122"/>
+      <c r="E49" s="121"/>
     </row>
     <row r="50" spans="5:5">
-      <c r="E50" s="122"/>
+      <c r="E50" s="121"/>
     </row>
     <row r="51" spans="5:5">
-      <c r="E51" s="122"/>
+      <c r="E51" s="121"/>
     </row>
     <row r="52" spans="5:5">
-      <c r="E52" s="122"/>
+      <c r="E52" s="121"/>
     </row>
     <row r="53" spans="5:5">
-      <c r="E53" s="122"/>
+      <c r="E53" s="121"/>
     </row>
     <row r="54" spans="5:5">
-      <c r="E54" s="122"/>
+      <c r="E54" s="121"/>
     </row>
     <row r="55" spans="5:5">
-      <c r="E55" s="122"/>
+      <c r="E55" s="121"/>
     </row>
     <row r="56" spans="5:5">
-      <c r="E56" s="122"/>
+      <c r="E56" s="121"/>
     </row>
     <row r="57" spans="5:5">
-      <c r="E57" s="122"/>
+      <c r="E57" s="121"/>
     </row>
     <row r="58" spans="5:5">
-      <c r="E58" s="122"/>
+      <c r="E58" s="121"/>
     </row>
     <row r="59" spans="5:5">
-      <c r="E59" s="122"/>
+      <c r="E59" s="121"/>
     </row>
     <row r="60" spans="5:5">
-      <c r="E60" s="122"/>
+      <c r="E60" s="121"/>
     </row>
     <row r="61" spans="5:5">
-      <c r="E61" s="122"/>
+      <c r="E61" s="121"/>
     </row>
   </sheetData>
   <sortState ref="A2:J11">
@@ -5423,8 +5420,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -5478,7 +5475,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="125" t="s">
+      <c r="A6" s="124" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="108" t="s">
@@ -5515,7 +5512,7 @@
       <c r="B13" s="108"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="113" t="s">
+      <c r="A14" s="124" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="109" t="s">
@@ -5529,13 +5526,13 @@
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="145" t="s">
+      <c r="C17" s="131" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="43" customFormat="1">
       <c r="A18" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B18" s="43" t="s">
         <v>6</v>
@@ -5543,15 +5540,15 @@
     </row>
     <row r="19" spans="1:3" s="67" customFormat="1">
       <c r="A19" s="99" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B19" s="79" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="125" t="s">
-        <v>106</v>
+      <c r="A20" s="124" t="s">
+        <v>103</v>
       </c>
       <c r="B20" s="106" t="s">
         <v>7</v>
@@ -5559,23 +5556,23 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="99" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B21" s="74" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="125" t="s">
-        <v>107</v>
+      <c r="A22" s="124" t="s">
+        <v>104</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="52" customFormat="1">
-      <c r="A23" s="125" t="s">
-        <v>107</v>
+      <c r="A23" s="124" t="s">
+        <v>104</v>
       </c>
       <c r="B23" s="52" t="s">
         <v>10</v>
@@ -5604,11 +5601,11 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="125" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="125" t="s">
-        <v>104</v>
+      <c r="A27" s="124" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="124" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -5618,17 +5615,17 @@
       <c r="B28" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="125" t="s">
+      <c r="C28" s="124" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="125"/>
-      <c r="B31" s="125"/>
+      <c r="A31" s="124"/>
+      <c r="B31" s="124"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B33" s="109" t="s">
         <v>25</v>
@@ -5636,24 +5633,24 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="99" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B34" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="125" t="s">
-        <v>94</v>
+      <c r="C34" s="124" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="99" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B35" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="125" t="s">
-        <v>94</v>
+      <c r="C35" s="124" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -5696,19 +5693,19 @@
   <sheetData>
     <row r="1" spans="1:12" s="48" customFormat="1">
       <c r="A1" s="48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J1" s="53"/>
       <c r="K1" s="51"/>
     </row>
     <row r="2" spans="1:12" s="48" customFormat="1">
-      <c r="E2" s="144" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
+      <c r="E2" s="146" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
       <c r="H2" s="49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I2" s="50">
         <v>0.45</v>
@@ -5718,34 +5715,34 @@
     </row>
     <row r="3" spans="1:12" ht="24">
       <c r="B3" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="E3" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="F3" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="G3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="J3" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3" s="54" t="s">
+      <c r="K3" s="51" t="s">
         <v>80</v>
-      </c>
-      <c r="J3" s="55" t="s">
-        <v>81</v>
-      </c>
-      <c r="K3" s="51" t="s">
-        <v>82</v>
       </c>
       <c r="L3" s="11" t="s">
         <v>2</v>
@@ -5753,7 +5750,7 @@
     </row>
     <row r="4" spans="1:12" s="59" customFormat="1">
       <c r="A4" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="60">
@@ -5799,7 +5796,7 @@
     </row>
     <row r="6" spans="1:12" s="59" customFormat="1">
       <c r="A6" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B6" s="11"/>
       <c r="E6" s="11"/>
@@ -5811,30 +5808,30 @@
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="137">
+      <c r="A7" s="139">
         <v>43692</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C7" s="98"/>
       <c r="D7" s="98"/>
       <c r="E7" s="98">
         <v>0</v>
       </c>
-      <c r="F7" s="138">
+      <c r="F7" s="140">
         <f>SUM(E7:E11)</f>
         <v>228</v>
       </c>
-      <c r="G7" s="138">
+      <c r="G7" s="140">
         <f>F7</f>
         <v>228</v>
       </c>
-      <c r="H7" s="139">
+      <c r="H7" s="141">
         <f>F7*$I$2</f>
         <v>102.60000000000001</v>
       </c>
-      <c r="I7" s="139">
+      <c r="I7" s="141">
         <f>H7</f>
         <v>102.60000000000001</v>
       </c>
@@ -5843,27 +5840,27 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="137"/>
+      <c r="A8" s="139"/>
       <c r="B8" s="99" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="98"/>
       <c r="D8" s="98"/>
       <c r="E8" s="98">
         <v>0</v>
       </c>
-      <c r="F8" s="138"/>
-      <c r="G8" s="138"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="139"/>
+      <c r="F8" s="140"/>
+      <c r="G8" s="140"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
       <c r="J8" s="100"/>
       <c r="K8" s="100"/>
       <c r="L8" s="77"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="137"/>
+      <c r="A9" s="139"/>
       <c r="B9" s="99" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" s="98">
         <v>81000</v>
@@ -5875,18 +5872,18 @@
       <c r="E9" s="98">
         <v>76</v>
       </c>
-      <c r="F9" s="138"/>
-      <c r="G9" s="138"/>
-      <c r="H9" s="139"/>
-      <c r="I9" s="139"/>
+      <c r="F9" s="140"/>
+      <c r="G9" s="140"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="141"/>
       <c r="J9" s="100"/>
       <c r="K9" s="100"/>
       <c r="L9" s="77"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="137"/>
+      <c r="A10" s="139"/>
       <c r="B10" s="99" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="98">
         <f>D9</f>
@@ -5899,18 +5896,18 @@
       <c r="E10" s="98">
         <v>76</v>
       </c>
-      <c r="F10" s="138"/>
-      <c r="G10" s="138"/>
-      <c r="H10" s="139"/>
-      <c r="I10" s="139"/>
+      <c r="F10" s="140"/>
+      <c r="G10" s="140"/>
+      <c r="H10" s="141"/>
+      <c r="I10" s="141"/>
       <c r="J10" s="100"/>
       <c r="K10" s="100"/>
       <c r="L10" s="77"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="137"/>
+      <c r="A11" s="139"/>
       <c r="B11" s="99" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11" s="98">
         <f t="shared" ref="C11:C31" si="1">D10</f>
@@ -5923,21 +5920,21 @@
       <c r="E11" s="98">
         <v>76</v>
       </c>
-      <c r="F11" s="138"/>
-      <c r="G11" s="138"/>
-      <c r="H11" s="139"/>
-      <c r="I11" s="139"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="141"/>
       <c r="J11" s="100"/>
       <c r="K11" s="100"/>
       <c r="L11" s="77"/>
     </row>
     <row r="12" spans="1:12" ht="10.5" customHeight="1">
-      <c r="A12" s="140">
+      <c r="A12" s="142">
         <f>A7+7</f>
         <v>43699</v>
       </c>
       <c r="B12" s="101" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12" s="102">
         <f t="shared" si="1"/>
@@ -5950,19 +5947,19 @@
       <c r="E12" s="102">
         <v>76</v>
       </c>
-      <c r="F12" s="141">
+      <c r="F12" s="143">
         <f>SUM(E12:E16)</f>
         <v>380</v>
       </c>
-      <c r="G12" s="141">
+      <c r="G12" s="143">
         <f>G7+F12</f>
         <v>608</v>
       </c>
-      <c r="H12" s="142">
+      <c r="H12" s="144">
         <f>F12*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I12" s="142">
+      <c r="I12" s="144">
         <f>I7+H12</f>
         <v>273.60000000000002</v>
       </c>
@@ -5971,9 +5968,9 @@
       <c r="L12" s="77"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="140"/>
+      <c r="A13" s="142"/>
       <c r="B13" s="101" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C13" s="102">
         <f t="shared" si="1"/>
@@ -5986,18 +5983,18 @@
       <c r="E13" s="102">
         <v>76</v>
       </c>
-      <c r="F13" s="141"/>
-      <c r="G13" s="141"/>
-      <c r="H13" s="142"/>
-      <c r="I13" s="142"/>
+      <c r="F13" s="143"/>
+      <c r="G13" s="143"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="144"/>
       <c r="J13" s="103"/>
       <c r="K13" s="103"/>
       <c r="L13" s="77"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="140"/>
+      <c r="A14" s="142"/>
       <c r="B14" s="101" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C14" s="102">
         <f t="shared" si="1"/>
@@ -6010,18 +6007,18 @@
       <c r="E14" s="102">
         <v>76</v>
       </c>
-      <c r="F14" s="141"/>
-      <c r="G14" s="141"/>
-      <c r="H14" s="142"/>
-      <c r="I14" s="142"/>
+      <c r="F14" s="143"/>
+      <c r="G14" s="143"/>
+      <c r="H14" s="144"/>
+      <c r="I14" s="144"/>
       <c r="J14" s="103"/>
       <c r="K14" s="103"/>
       <c r="L14" s="77"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="140"/>
+      <c r="A15" s="142"/>
       <c r="B15" s="101" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C15" s="102">
         <f t="shared" si="1"/>
@@ -6034,18 +6031,18 @@
       <c r="E15" s="102">
         <v>76</v>
       </c>
-      <c r="F15" s="141"/>
-      <c r="G15" s="141"/>
-      <c r="H15" s="142"/>
-      <c r="I15" s="142"/>
+      <c r="F15" s="143"/>
+      <c r="G15" s="143"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="144"/>
       <c r="J15" s="103"/>
       <c r="K15" s="103"/>
       <c r="L15" s="77"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="140"/>
+      <c r="A16" s="142"/>
       <c r="B16" s="101" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C16" s="102">
         <f t="shared" si="1"/>
@@ -6058,38 +6055,38 @@
       <c r="E16" s="102">
         <v>76</v>
       </c>
-      <c r="F16" s="141"/>
-      <c r="G16" s="141"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
+      <c r="F16" s="143"/>
+      <c r="G16" s="143"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
       <c r="J16" s="103"/>
       <c r="K16" s="103"/>
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="137">
+      <c r="A17" s="139">
         <f>A12+7</f>
         <v>43706</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17" s="98"/>
       <c r="D17" s="98"/>
       <c r="E17" s="98"/>
-      <c r="F17" s="138">
+      <c r="F17" s="140">
         <f>SUM(E17:E21)</f>
         <v>304</v>
       </c>
-      <c r="G17" s="138">
+      <c r="G17" s="140">
         <f>G12+F17</f>
         <v>912</v>
       </c>
-      <c r="H17" s="139">
+      <c r="H17" s="141">
         <f>F17*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I17" s="139">
+      <c r="I17" s="141">
         <f>I12+H17</f>
         <v>410.40000000000003</v>
       </c>
@@ -6098,9 +6095,9 @@
       <c r="L17" s="77"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="137"/>
+      <c r="A18" s="139"/>
       <c r="B18" s="99" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C18" s="98">
         <f>D16</f>
@@ -6113,18 +6110,18 @@
       <c r="E18" s="98">
         <v>76</v>
       </c>
-      <c r="F18" s="138"/>
-      <c r="G18" s="138"/>
-      <c r="H18" s="139"/>
-      <c r="I18" s="139"/>
+      <c r="F18" s="140"/>
+      <c r="G18" s="140"/>
+      <c r="H18" s="141"/>
+      <c r="I18" s="141"/>
       <c r="J18" s="100"/>
       <c r="K18" s="100"/>
       <c r="L18" s="77"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="137"/>
+      <c r="A19" s="139"/>
       <c r="B19" s="99" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C19" s="98">
         <f t="shared" si="1"/>
@@ -6137,18 +6134,18 @@
       <c r="E19" s="98">
         <v>76</v>
       </c>
-      <c r="F19" s="138"/>
-      <c r="G19" s="138"/>
-      <c r="H19" s="139"/>
-      <c r="I19" s="139"/>
+      <c r="F19" s="140"/>
+      <c r="G19" s="140"/>
+      <c r="H19" s="141"/>
+      <c r="I19" s="141"/>
       <c r="J19" s="100"/>
       <c r="K19" s="100"/>
       <c r="L19" s="77"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="137"/>
+      <c r="A20" s="139"/>
       <c r="B20" s="99" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" s="98">
         <f t="shared" si="1"/>
@@ -6161,18 +6158,18 @@
       <c r="E20" s="98">
         <v>76</v>
       </c>
-      <c r="F20" s="138"/>
-      <c r="G20" s="138"/>
-      <c r="H20" s="139"/>
-      <c r="I20" s="139"/>
+      <c r="F20" s="140"/>
+      <c r="G20" s="140"/>
+      <c r="H20" s="141"/>
+      <c r="I20" s="141"/>
       <c r="J20" s="100"/>
       <c r="K20" s="100"/>
       <c r="L20" s="77"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="137"/>
+      <c r="A21" s="139"/>
       <c r="B21" s="99" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C21" s="98">
         <f t="shared" si="1"/>
@@ -6185,21 +6182,21 @@
       <c r="E21" s="98">
         <v>76</v>
       </c>
-      <c r="F21" s="138"/>
-      <c r="G21" s="138"/>
-      <c r="H21" s="139"/>
-      <c r="I21" s="139"/>
+      <c r="F21" s="140"/>
+      <c r="G21" s="140"/>
+      <c r="H21" s="141"/>
+      <c r="I21" s="141"/>
       <c r="J21" s="100"/>
       <c r="K21" s="100"/>
       <c r="L21" s="77"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="140">
+      <c r="A22" s="142">
         <f>A17+7</f>
         <v>43713</v>
       </c>
       <c r="B22" s="101" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22" s="102">
         <f t="shared" si="1"/>
@@ -6212,19 +6209,19 @@
       <c r="E22" s="102">
         <v>76</v>
       </c>
-      <c r="F22" s="141">
+      <c r="F22" s="143">
         <f>SUM(E22:E26)</f>
         <v>380</v>
       </c>
-      <c r="G22" s="141">
+      <c r="G22" s="143">
         <f>G17+F22</f>
         <v>1292</v>
       </c>
-      <c r="H22" s="142">
+      <c r="H22" s="144">
         <f>F22*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I22" s="142">
+      <c r="I22" s="144">
         <f>I17+H22</f>
         <v>581.40000000000009</v>
       </c>
@@ -6233,9 +6230,9 @@
       <c r="L22" s="11"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="140"/>
+      <c r="A23" s="142"/>
       <c r="B23" s="101" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C23" s="102">
         <f t="shared" si="1"/>
@@ -6248,18 +6245,18 @@
       <c r="E23" s="102">
         <v>76</v>
       </c>
-      <c r="F23" s="141"/>
-      <c r="G23" s="141"/>
-      <c r="H23" s="142"/>
-      <c r="I23" s="142"/>
+      <c r="F23" s="143"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="144"/>
+      <c r="I23" s="144"/>
       <c r="J23" s="103"/>
       <c r="K23" s="103"/>
       <c r="L23" s="77"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="140"/>
+      <c r="A24" s="142"/>
       <c r="B24" s="101" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C24" s="102">
         <f t="shared" si="1"/>
@@ -6272,18 +6269,18 @@
       <c r="E24" s="102">
         <v>76</v>
       </c>
-      <c r="F24" s="141"/>
-      <c r="G24" s="141"/>
-      <c r="H24" s="142"/>
-      <c r="I24" s="142"/>
+      <c r="F24" s="143"/>
+      <c r="G24" s="143"/>
+      <c r="H24" s="144"/>
+      <c r="I24" s="144"/>
       <c r="J24" s="103"/>
       <c r="K24" s="103"/>
       <c r="L24" s="77"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="140"/>
+      <c r="A25" s="142"/>
       <c r="B25" s="101" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C25" s="102">
         <f t="shared" si="1"/>
@@ -6296,18 +6293,18 @@
       <c r="E25" s="102">
         <v>76</v>
       </c>
-      <c r="F25" s="141"/>
-      <c r="G25" s="141"/>
-      <c r="H25" s="142"/>
-      <c r="I25" s="142"/>
+      <c r="F25" s="143"/>
+      <c r="G25" s="143"/>
+      <c r="H25" s="144"/>
+      <c r="I25" s="144"/>
       <c r="J25" s="103"/>
       <c r="K25" s="103"/>
       <c r="L25" s="77"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="140"/>
+      <c r="A26" s="142"/>
       <c r="B26" s="101" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C26" s="102">
         <f t="shared" si="1"/>
@@ -6320,21 +6317,21 @@
       <c r="E26" s="102">
         <v>76</v>
       </c>
-      <c r="F26" s="141"/>
-      <c r="G26" s="141"/>
-      <c r="H26" s="142"/>
-      <c r="I26" s="142"/>
+      <c r="F26" s="143"/>
+      <c r="G26" s="143"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="144"/>
       <c r="J26" s="103"/>
       <c r="K26" s="103"/>
       <c r="L26" s="77"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="137">
+      <c r="A27" s="139">
         <f>A22+7</f>
         <v>43720</v>
       </c>
       <c r="B27" s="99" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C27" s="98">
         <f t="shared" si="1"/>
@@ -6347,19 +6344,19 @@
       <c r="E27" s="98">
         <v>76</v>
       </c>
-      <c r="F27" s="138">
+      <c r="F27" s="140">
         <f>SUM(E27:E31)</f>
         <v>380</v>
       </c>
-      <c r="G27" s="138">
+      <c r="G27" s="140">
         <f>G22+F27</f>
         <v>1672</v>
       </c>
-      <c r="H27" s="139">
+      <c r="H27" s="141">
         <f>F27*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I27" s="139">
+      <c r="I27" s="141">
         <f>I22+H27</f>
         <v>752.40000000000009</v>
       </c>
@@ -6368,9 +6365,9 @@
       <c r="L27" s="77"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="137"/>
+      <c r="A28" s="139"/>
       <c r="B28" s="99" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C28" s="98">
         <f t="shared" si="1"/>
@@ -6383,18 +6380,18 @@
       <c r="E28" s="98">
         <v>76</v>
       </c>
-      <c r="F28" s="138"/>
-      <c r="G28" s="138"/>
-      <c r="H28" s="139"/>
-      <c r="I28" s="139"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="141"/>
+      <c r="I28" s="141"/>
       <c r="J28" s="100"/>
       <c r="K28" s="100"/>
       <c r="L28" s="77"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="137"/>
+      <c r="A29" s="139"/>
       <c r="B29" s="99" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C29" s="98">
         <f t="shared" si="1"/>
@@ -6407,18 +6404,18 @@
       <c r="E29" s="98">
         <v>76</v>
       </c>
-      <c r="F29" s="138"/>
-      <c r="G29" s="138"/>
-      <c r="H29" s="139"/>
-      <c r="I29" s="139"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="141"/>
+      <c r="I29" s="141"/>
       <c r="J29" s="100"/>
       <c r="K29" s="100"/>
       <c r="L29" s="77"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="137"/>
+      <c r="A30" s="139"/>
       <c r="B30" s="99" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C30" s="98">
         <f t="shared" si="1"/>
@@ -6431,18 +6428,18 @@
       <c r="E30" s="98">
         <v>76</v>
       </c>
-      <c r="F30" s="138"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="139"/>
-      <c r="I30" s="139"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="141"/>
+      <c r="I30" s="141"/>
       <c r="J30" s="100"/>
       <c r="K30" s="100"/>
       <c r="L30" s="77"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="137"/>
+      <c r="A31" s="139"/>
       <c r="B31" s="99" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C31" s="98">
         <f t="shared" si="1"/>
@@ -6455,53 +6452,53 @@
       <c r="E31" s="98">
         <v>76</v>
       </c>
-      <c r="F31" s="138"/>
-      <c r="G31" s="138"/>
-      <c r="H31" s="139"/>
-      <c r="I31" s="139"/>
+      <c r="F31" s="140"/>
+      <c r="G31" s="140"/>
+      <c r="H31" s="141"/>
+      <c r="I31" s="141"/>
       <c r="J31" s="100"/>
       <c r="K31" s="100"/>
       <c r="L31" s="77"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="140">
+      <c r="A32" s="142">
         <f>A27+7</f>
         <v>43727</v>
       </c>
       <c r="B32" s="101" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C32" s="102"/>
       <c r="D32" s="102"/>
       <c r="E32" s="102">
         <v>0</v>
       </c>
-      <c r="F32" s="143">
+      <c r="F32" s="145">
         <f>SUM(E32:E36)</f>
         <v>304</v>
       </c>
-      <c r="G32" s="143">
+      <c r="G32" s="145">
         <f>G27+F32</f>
         <v>1976</v>
       </c>
-      <c r="H32" s="142">
+      <c r="H32" s="144">
         <f>F32*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I32" s="142">
+      <c r="I32" s="144">
         <f>I27+H32</f>
         <v>889.2</v>
       </c>
       <c r="J32" s="103"/>
       <c r="K32" s="103"/>
-      <c r="L32" s="124" t="s">
-        <v>90</v>
+      <c r="L32" s="123" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="140"/>
+      <c r="A33" s="142"/>
       <c r="B33" s="101" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33" s="102">
         <f>D31</f>
@@ -6514,17 +6511,17 @@
       <c r="E33" s="102">
         <v>76</v>
       </c>
-      <c r="F33" s="143"/>
-      <c r="G33" s="143"/>
-      <c r="H33" s="142"/>
-      <c r="I33" s="142"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145"/>
+      <c r="H33" s="144"/>
+      <c r="I33" s="144"/>
       <c r="J33" s="103"/>
       <c r="K33" s="103"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="140"/>
+      <c r="A34" s="142"/>
       <c r="B34" s="101" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C34" s="102">
         <f t="shared" ref="C34:C50" si="3">D33</f>
@@ -6537,17 +6534,17 @@
       <c r="E34" s="102">
         <v>76</v>
       </c>
-      <c r="F34" s="143"/>
-      <c r="G34" s="143"/>
-      <c r="H34" s="142"/>
-      <c r="I34" s="142"/>
+      <c r="F34" s="145"/>
+      <c r="G34" s="145"/>
+      <c r="H34" s="144"/>
+      <c r="I34" s="144"/>
       <c r="J34" s="103"/>
       <c r="K34" s="103"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="140"/>
+      <c r="A35" s="142"/>
       <c r="B35" s="101" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C35" s="102">
         <f t="shared" si="3"/>
@@ -6560,17 +6557,17 @@
       <c r="E35" s="102">
         <v>76</v>
       </c>
-      <c r="F35" s="143"/>
-      <c r="G35" s="143"/>
-      <c r="H35" s="142"/>
-      <c r="I35" s="142"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="145"/>
+      <c r="H35" s="144"/>
+      <c r="I35" s="144"/>
       <c r="J35" s="103"/>
       <c r="K35" s="103"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="140"/>
+      <c r="A36" s="142"/>
       <c r="B36" s="101" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C36" s="102">
         <f t="shared" si="3"/>
@@ -6583,20 +6580,20 @@
       <c r="E36" s="102">
         <v>76</v>
       </c>
-      <c r="F36" s="143"/>
-      <c r="G36" s="143"/>
-      <c r="H36" s="142"/>
-      <c r="I36" s="142"/>
+      <c r="F36" s="145"/>
+      <c r="G36" s="145"/>
+      <c r="H36" s="144"/>
+      <c r="I36" s="144"/>
       <c r="J36" s="103"/>
       <c r="K36" s="103"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="137">
+      <c r="A37" s="139">
         <f>A32+7</f>
         <v>43734</v>
       </c>
       <c r="B37" s="99" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C37" s="98">
         <f t="shared" si="3"/>
@@ -6609,19 +6606,19 @@
       <c r="E37" s="98">
         <v>76</v>
       </c>
-      <c r="F37" s="138">
+      <c r="F37" s="140">
         <f>SUM(E37:E41)</f>
         <v>380</v>
       </c>
-      <c r="G37" s="138">
+      <c r="G37" s="140">
         <f>G32+F37</f>
         <v>2356</v>
       </c>
-      <c r="H37" s="139">
+      <c r="H37" s="141">
         <f>F37*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I37" s="139">
+      <c r="I37" s="141">
         <f>I32+H37</f>
         <v>1060.2</v>
       </c>
@@ -6629,9 +6626,9 @@
       <c r="K37" s="100"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="137"/>
+      <c r="A38" s="139"/>
       <c r="B38" s="99" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C38" s="98">
         <f t="shared" si="3"/>
@@ -6644,17 +6641,17 @@
       <c r="E38" s="98">
         <v>76</v>
       </c>
-      <c r="F38" s="138"/>
-      <c r="G38" s="138"/>
-      <c r="H38" s="139"/>
-      <c r="I38" s="139"/>
+      <c r="F38" s="140"/>
+      <c r="G38" s="140"/>
+      <c r="H38" s="141"/>
+      <c r="I38" s="141"/>
       <c r="J38" s="100"/>
       <c r="K38" s="100"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="137"/>
+      <c r="A39" s="139"/>
       <c r="B39" s="99" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C39" s="98">
         <f t="shared" si="3"/>
@@ -6667,17 +6664,17 @@
       <c r="E39" s="98">
         <v>76</v>
       </c>
-      <c r="F39" s="138"/>
-      <c r="G39" s="138"/>
-      <c r="H39" s="139"/>
-      <c r="I39" s="139"/>
+      <c r="F39" s="140"/>
+      <c r="G39" s="140"/>
+      <c r="H39" s="141"/>
+      <c r="I39" s="141"/>
       <c r="J39" s="100"/>
       <c r="K39" s="100"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="137"/>
+      <c r="A40" s="139"/>
       <c r="B40" s="99" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C40" s="98">
         <f t="shared" si="3"/>
@@ -6690,17 +6687,17 @@
       <c r="E40" s="98">
         <v>76</v>
       </c>
-      <c r="F40" s="138"/>
-      <c r="G40" s="138"/>
-      <c r="H40" s="139"/>
-      <c r="I40" s="139"/>
+      <c r="F40" s="140"/>
+      <c r="G40" s="140"/>
+      <c r="H40" s="141"/>
+      <c r="I40" s="141"/>
       <c r="J40" s="100"/>
       <c r="K40" s="100"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="137"/>
+      <c r="A41" s="139"/>
       <c r="B41" s="99" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C41" s="98">
         <f t="shared" si="3"/>
@@ -6713,20 +6710,20 @@
       <c r="E41" s="98">
         <v>76</v>
       </c>
-      <c r="F41" s="138"/>
-      <c r="G41" s="138"/>
-      <c r="H41" s="139"/>
-      <c r="I41" s="139"/>
+      <c r="F41" s="140"/>
+      <c r="G41" s="140"/>
+      <c r="H41" s="141"/>
+      <c r="I41" s="141"/>
       <c r="J41" s="100"/>
       <c r="K41" s="100"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="140">
+      <c r="A42" s="142">
         <f>A37+7</f>
         <v>43741</v>
       </c>
       <c r="B42" s="101" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C42" s="102">
         <f t="shared" si="3"/>
@@ -6739,19 +6736,19 @@
       <c r="E42" s="102">
         <v>76</v>
       </c>
-      <c r="F42" s="143">
+      <c r="F42" s="145">
         <f>SUM(E42:E46)</f>
         <v>304</v>
       </c>
-      <c r="G42" s="143">
+      <c r="G42" s="145">
         <f>G37+F42</f>
         <v>2660</v>
       </c>
-      <c r="H42" s="142">
+      <c r="H42" s="144">
         <f>F42*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I42" s="142">
+      <c r="I42" s="144">
         <f>I37+H42</f>
         <v>1197</v>
       </c>
@@ -6759,9 +6756,9 @@
       <c r="K42" s="103"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="140"/>
+      <c r="A43" s="142"/>
       <c r="B43" s="101" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C43" s="102">
         <f t="shared" si="3"/>
@@ -6774,17 +6771,17 @@
       <c r="E43" s="102">
         <v>76</v>
       </c>
-      <c r="F43" s="143"/>
-      <c r="G43" s="143"/>
-      <c r="H43" s="142"/>
-      <c r="I43" s="142"/>
+      <c r="F43" s="145"/>
+      <c r="G43" s="145"/>
+      <c r="H43" s="144"/>
+      <c r="I43" s="144"/>
       <c r="J43" s="103"/>
       <c r="K43" s="103"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="140"/>
+      <c r="A44" s="142"/>
       <c r="B44" s="101" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44" s="102">
         <f t="shared" si="3"/>
@@ -6797,17 +6794,17 @@
       <c r="E44" s="102">
         <v>76</v>
       </c>
-      <c r="F44" s="143"/>
-      <c r="G44" s="143"/>
-      <c r="H44" s="142"/>
-      <c r="I44" s="142"/>
+      <c r="F44" s="145"/>
+      <c r="G44" s="145"/>
+      <c r="H44" s="144"/>
+      <c r="I44" s="144"/>
       <c r="J44" s="103"/>
       <c r="K44" s="103"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="140"/>
+      <c r="A45" s="142"/>
       <c r="B45" s="101" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C45" s="102">
         <f t="shared" si="3"/>
@@ -6820,72 +6817,72 @@
       <c r="E45" s="102">
         <v>76</v>
       </c>
-      <c r="F45" s="143"/>
-      <c r="G45" s="143"/>
-      <c r="H45" s="142"/>
-      <c r="I45" s="142"/>
+      <c r="F45" s="145"/>
+      <c r="G45" s="145"/>
+      <c r="H45" s="144"/>
+      <c r="I45" s="144"/>
       <c r="J45" s="103"/>
       <c r="K45" s="103"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="140"/>
+      <c r="A46" s="142"/>
       <c r="B46" s="101" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C46" s="102"/>
       <c r="D46" s="102"/>
       <c r="E46" s="102">
         <v>0</v>
       </c>
-      <c r="F46" s="143"/>
-      <c r="G46" s="143"/>
-      <c r="H46" s="142"/>
-      <c r="I46" s="142"/>
+      <c r="F46" s="145"/>
+      <c r="G46" s="145"/>
+      <c r="H46" s="144"/>
+      <c r="I46" s="144"/>
       <c r="J46" s="103"/>
       <c r="K46" s="103"/>
-      <c r="L46" s="124" t="s">
-        <v>91</v>
+      <c r="L46" s="123" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="137">
+      <c r="A47" s="139">
         <f>A42+7</f>
         <v>43748</v>
       </c>
       <c r="B47" s="99" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C47" s="98"/>
       <c r="D47" s="98"/>
       <c r="E47" s="98">
         <v>0</v>
       </c>
-      <c r="F47" s="138">
+      <c r="F47" s="140">
         <f>SUM(E47:E51)</f>
         <v>304</v>
       </c>
-      <c r="G47" s="138">
+      <c r="G47" s="140">
         <f>G42+F47</f>
         <v>2964</v>
       </c>
-      <c r="H47" s="139">
+      <c r="H47" s="141">
         <f>F47*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I47" s="139">
+      <c r="I47" s="141">
         <f>I42+H47</f>
         <v>1333.8</v>
       </c>
       <c r="J47" s="100"/>
       <c r="K47" s="100"/>
-      <c r="L47" s="124" t="s">
-        <v>91</v>
+      <c r="L47" s="123" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="137"/>
+      <c r="A48" s="139"/>
       <c r="B48" s="99" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C48" s="98">
         <f>D45</f>
@@ -6898,17 +6895,17 @@
       <c r="E48" s="98">
         <v>76</v>
       </c>
-      <c r="F48" s="138"/>
-      <c r="G48" s="138"/>
-      <c r="H48" s="139"/>
-      <c r="I48" s="139"/>
+      <c r="F48" s="140"/>
+      <c r="G48" s="140"/>
+      <c r="H48" s="141"/>
+      <c r="I48" s="141"/>
       <c r="J48" s="100"/>
       <c r="K48" s="100"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="137"/>
+      <c r="A49" s="139"/>
       <c r="B49" s="99" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C49" s="98">
         <f t="shared" si="3"/>
@@ -6921,17 +6918,17 @@
       <c r="E49" s="98">
         <v>76</v>
       </c>
-      <c r="F49" s="138"/>
-      <c r="G49" s="138"/>
-      <c r="H49" s="139"/>
-      <c r="I49" s="139"/>
+      <c r="F49" s="140"/>
+      <c r="G49" s="140"/>
+      <c r="H49" s="141"/>
+      <c r="I49" s="141"/>
       <c r="J49" s="100"/>
       <c r="K49" s="100"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="137"/>
+      <c r="A50" s="139"/>
       <c r="B50" s="99" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C50" s="98">
         <f t="shared" si="3"/>
@@ -6944,17 +6941,17 @@
       <c r="E50" s="98">
         <v>76</v>
       </c>
-      <c r="F50" s="138"/>
-      <c r="G50" s="138"/>
-      <c r="H50" s="139"/>
-      <c r="I50" s="139"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="140"/>
+      <c r="H50" s="141"/>
+      <c r="I50" s="141"/>
       <c r="J50" s="100"/>
       <c r="K50" s="100"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="137"/>
+      <c r="A51" s="139"/>
       <c r="B51" s="99" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C51" s="98">
         <f>D50</f>
@@ -6967,32 +6964,32 @@
       <c r="E51" s="98">
         <v>76</v>
       </c>
-      <c r="F51" s="138"/>
-      <c r="G51" s="138"/>
-      <c r="H51" s="139"/>
-      <c r="I51" s="139"/>
+      <c r="F51" s="140"/>
+      <c r="G51" s="140"/>
+      <c r="H51" s="141"/>
+      <c r="I51" s="141"/>
       <c r="J51" s="100"/>
       <c r="K51" s="100"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="140"/>
+      <c r="A52" s="142"/>
       <c r="B52" s="101"/>
       <c r="C52" s="102"/>
       <c r="D52" s="102"/>
       <c r="E52" s="102"/>
-      <c r="F52" s="143">
+      <c r="F52" s="145">
         <f>SUM(E52:E56)</f>
         <v>0</v>
       </c>
-      <c r="G52" s="143">
+      <c r="G52" s="145">
         <f>G47+F52</f>
         <v>2964</v>
       </c>
-      <c r="H52" s="142">
+      <c r="H52" s="144">
         <f>F52*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I52" s="142">
+      <c r="I52" s="144">
         <f>I47+H52</f>
         <v>1333.8</v>
       </c>
@@ -7000,76 +6997,76 @@
       <c r="K52" s="103"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="140"/>
+      <c r="A53" s="142"/>
       <c r="B53" s="101"/>
       <c r="C53" s="102"/>
       <c r="D53" s="102"/>
       <c r="E53" s="102"/>
-      <c r="F53" s="143"/>
-      <c r="G53" s="143"/>
-      <c r="H53" s="142"/>
-      <c r="I53" s="142"/>
+      <c r="F53" s="145"/>
+      <c r="G53" s="145"/>
+      <c r="H53" s="144"/>
+      <c r="I53" s="144"/>
       <c r="J53" s="103"/>
       <c r="K53" s="103"/>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="140"/>
+      <c r="A54" s="142"/>
       <c r="B54" s="101"/>
       <c r="C54" s="102"/>
       <c r="D54" s="102"/>
       <c r="E54" s="102"/>
-      <c r="F54" s="143"/>
-      <c r="G54" s="143"/>
-      <c r="H54" s="142"/>
-      <c r="I54" s="142"/>
+      <c r="F54" s="145"/>
+      <c r="G54" s="145"/>
+      <c r="H54" s="144"/>
+      <c r="I54" s="144"/>
       <c r="J54" s="103"/>
       <c r="K54" s="103"/>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="140"/>
+      <c r="A55" s="142"/>
       <c r="B55" s="101"/>
       <c r="C55" s="102"/>
       <c r="D55" s="102"/>
       <c r="E55" s="102"/>
-      <c r="F55" s="143"/>
-      <c r="G55" s="143"/>
-      <c r="H55" s="142"/>
-      <c r="I55" s="142"/>
+      <c r="F55" s="145"/>
+      <c r="G55" s="145"/>
+      <c r="H55" s="144"/>
+      <c r="I55" s="144"/>
       <c r="J55" s="103"/>
       <c r="K55" s="103"/>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="140"/>
+      <c r="A56" s="142"/>
       <c r="B56" s="101"/>
       <c r="C56" s="102"/>
       <c r="D56" s="102"/>
       <c r="E56" s="102"/>
-      <c r="F56" s="143"/>
-      <c r="G56" s="143"/>
-      <c r="H56" s="142"/>
-      <c r="I56" s="142"/>
+      <c r="F56" s="145"/>
+      <c r="G56" s="145"/>
+      <c r="H56" s="144"/>
+      <c r="I56" s="144"/>
       <c r="J56" s="103"/>
       <c r="K56" s="103"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="137"/>
+      <c r="A57" s="139"/>
       <c r="B57" s="99"/>
       <c r="C57" s="98"/>
       <c r="D57" s="98"/>
       <c r="E57" s="98"/>
-      <c r="F57" s="138">
+      <c r="F57" s="140">
         <f>SUM(E57:E61)</f>
         <v>0</v>
       </c>
-      <c r="G57" s="138">
+      <c r="G57" s="140">
         <f>G52+F57</f>
         <v>2964</v>
       </c>
-      <c r="H57" s="139">
+      <c r="H57" s="141">
         <f>F57*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I57" s="139">
+      <c r="I57" s="141">
         <f>I52+H57</f>
         <v>1333.8</v>
       </c>
@@ -7077,76 +7074,76 @@
       <c r="K57" s="100"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="137"/>
+      <c r="A58" s="139"/>
       <c r="B58" s="99"/>
       <c r="C58" s="98"/>
       <c r="D58" s="98"/>
       <c r="E58" s="98"/>
-      <c r="F58" s="138"/>
-      <c r="G58" s="138"/>
-      <c r="H58" s="139"/>
-      <c r="I58" s="139"/>
+      <c r="F58" s="140"/>
+      <c r="G58" s="140"/>
+      <c r="H58" s="141"/>
+      <c r="I58" s="141"/>
       <c r="J58" s="100"/>
       <c r="K58" s="100"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="137"/>
+      <c r="A59" s="139"/>
       <c r="B59" s="99"/>
       <c r="C59" s="98"/>
       <c r="D59" s="98"/>
       <c r="E59" s="98"/>
-      <c r="F59" s="138"/>
-      <c r="G59" s="138"/>
-      <c r="H59" s="139"/>
-      <c r="I59" s="139"/>
+      <c r="F59" s="140"/>
+      <c r="G59" s="140"/>
+      <c r="H59" s="141"/>
+      <c r="I59" s="141"/>
       <c r="J59" s="100"/>
       <c r="K59" s="100"/>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="137"/>
+      <c r="A60" s="139"/>
       <c r="B60" s="99"/>
       <c r="C60" s="98"/>
       <c r="D60" s="98"/>
       <c r="E60" s="98"/>
-      <c r="F60" s="138"/>
-      <c r="G60" s="138"/>
-      <c r="H60" s="139"/>
-      <c r="I60" s="139"/>
+      <c r="F60" s="140"/>
+      <c r="G60" s="140"/>
+      <c r="H60" s="141"/>
+      <c r="I60" s="141"/>
       <c r="J60" s="100"/>
       <c r="K60" s="100"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="137"/>
+      <c r="A61" s="139"/>
       <c r="B61" s="99"/>
       <c r="C61" s="98"/>
       <c r="D61" s="98"/>
       <c r="E61" s="98"/>
-      <c r="F61" s="138"/>
-      <c r="G61" s="138"/>
-      <c r="H61" s="139"/>
-      <c r="I61" s="139"/>
+      <c r="F61" s="140"/>
+      <c r="G61" s="140"/>
+      <c r="H61" s="141"/>
+      <c r="I61" s="141"/>
       <c r="J61" s="100"/>
       <c r="K61" s="100"/>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="140"/>
+      <c r="A62" s="142"/>
       <c r="B62" s="101"/>
       <c r="C62" s="102"/>
       <c r="D62" s="102"/>
       <c r="E62" s="102"/>
-      <c r="F62" s="143">
+      <c r="F62" s="145">
         <f>SUM(E62:E66)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="143">
+      <c r="G62" s="145">
         <f>G57+F62</f>
         <v>2964</v>
       </c>
-      <c r="H62" s="142">
+      <c r="H62" s="144">
         <f>F62*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I62" s="142">
+      <c r="I62" s="144">
         <f>I57+H62</f>
         <v>1333.8</v>
       </c>
@@ -7154,54 +7151,54 @@
       <c r="K62" s="103"/>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="140"/>
+      <c r="A63" s="142"/>
       <c r="B63" s="101"/>
       <c r="C63" s="102"/>
       <c r="D63" s="102"/>
       <c r="E63" s="102"/>
-      <c r="F63" s="143"/>
-      <c r="G63" s="143"/>
-      <c r="H63" s="142"/>
-      <c r="I63" s="142"/>
+      <c r="F63" s="145"/>
+      <c r="G63" s="145"/>
+      <c r="H63" s="144"/>
+      <c r="I63" s="144"/>
       <c r="J63" s="103"/>
       <c r="K63" s="103"/>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="140"/>
+      <c r="A64" s="142"/>
       <c r="B64" s="101"/>
       <c r="C64" s="102"/>
       <c r="D64" s="102"/>
       <c r="E64" s="102"/>
-      <c r="F64" s="143"/>
-      <c r="G64" s="143"/>
-      <c r="H64" s="142"/>
-      <c r="I64" s="142"/>
+      <c r="F64" s="145"/>
+      <c r="G64" s="145"/>
+      <c r="H64" s="144"/>
+      <c r="I64" s="144"/>
       <c r="J64" s="103"/>
       <c r="K64" s="103"/>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="140"/>
+      <c r="A65" s="142"/>
       <c r="B65" s="101"/>
       <c r="C65" s="102"/>
       <c r="D65" s="102"/>
       <c r="E65" s="102"/>
-      <c r="F65" s="143"/>
-      <c r="G65" s="143"/>
-      <c r="H65" s="142"/>
-      <c r="I65" s="142"/>
+      <c r="F65" s="145"/>
+      <c r="G65" s="145"/>
+      <c r="H65" s="144"/>
+      <c r="I65" s="144"/>
       <c r="J65" s="103"/>
       <c r="K65" s="103"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="140"/>
+      <c r="A66" s="142"/>
       <c r="B66" s="101"/>
       <c r="C66" s="102"/>
       <c r="D66" s="102"/>
       <c r="E66" s="102"/>
-      <c r="F66" s="143"/>
-      <c r="G66" s="143"/>
-      <c r="H66" s="142"/>
-      <c r="I66" s="142"/>
+      <c r="F66" s="145"/>
+      <c r="G66" s="145"/>
+      <c r="H66" s="144"/>
+      <c r="I66" s="144"/>
       <c r="J66" s="103"/>
       <c r="K66" s="103"/>
     </row>

</xml_diff>

<commit_message>
Current account category now handles credit cards
</commit_message>
<xml_diff>
--- a/Lava3.Test/TestFiles/Test.xlsx
+++ b/Lava3.Test/TestFiles/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="585" windowWidth="15555" windowHeight="18030" tabRatio="554" activeTab="1"/>
+    <workbookView xWindow="510" yWindow="585" windowWidth="15555" windowHeight="18030" tabRatio="554" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Annual Summary" sheetId="2" r:id="rId1"/>
@@ -2194,6 +2194,15 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2203,20 +2212,11 @@
     <xf numFmtId="44" fontId="20" fillId="0" borderId="0" xfId="763" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="931">
@@ -4791,7 +4791,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
@@ -5002,9 +5002,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -5066,7 +5066,7 @@
         <v>45</v>
       </c>
       <c r="E2" s="120">
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="F2" s="122"/>
       <c r="G2" s="74">
@@ -5699,11 +5699,11 @@
       <c r="K1" s="51"/>
     </row>
     <row r="2" spans="1:12" s="48" customFormat="1">
-      <c r="E2" s="146" t="s">
+      <c r="E2" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
       <c r="H2" s="49" t="s">
         <v>72</v>
       </c>
@@ -5808,7 +5808,7 @@
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="139">
+      <c r="A7" s="142">
         <v>43692</v>
       </c>
       <c r="B7" s="99" t="s">
@@ -5819,19 +5819,19 @@
       <c r="E7" s="98">
         <v>0</v>
       </c>
-      <c r="F7" s="140">
+      <c r="F7" s="143">
         <f>SUM(E7:E11)</f>
         <v>228</v>
       </c>
-      <c r="G7" s="140">
+      <c r="G7" s="143">
         <f>F7</f>
         <v>228</v>
       </c>
-      <c r="H7" s="141">
+      <c r="H7" s="144">
         <f>F7*$I$2</f>
         <v>102.60000000000001</v>
       </c>
-      <c r="I7" s="141">
+      <c r="I7" s="144">
         <f>H7</f>
         <v>102.60000000000001</v>
       </c>
@@ -5840,7 +5840,7 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="139"/>
+      <c r="A8" s="142"/>
       <c r="B8" s="99" t="s">
         <v>84</v>
       </c>
@@ -5849,16 +5849,16 @@
       <c r="E8" s="98">
         <v>0</v>
       </c>
-      <c r="F8" s="140"/>
-      <c r="G8" s="140"/>
-      <c r="H8" s="141"/>
-      <c r="I8" s="141"/>
+      <c r="F8" s="143"/>
+      <c r="G8" s="143"/>
+      <c r="H8" s="144"/>
+      <c r="I8" s="144"/>
       <c r="J8" s="100"/>
       <c r="K8" s="100"/>
       <c r="L8" s="77"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="139"/>
+      <c r="A9" s="142"/>
       <c r="B9" s="99" t="s">
         <v>85</v>
       </c>
@@ -5872,16 +5872,16 @@
       <c r="E9" s="98">
         <v>76</v>
       </c>
-      <c r="F9" s="140"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="141"/>
-      <c r="I9" s="141"/>
+      <c r="F9" s="143"/>
+      <c r="G9" s="143"/>
+      <c r="H9" s="144"/>
+      <c r="I9" s="144"/>
       <c r="J9" s="100"/>
       <c r="K9" s="100"/>
       <c r="L9" s="77"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="139"/>
+      <c r="A10" s="142"/>
       <c r="B10" s="99" t="s">
         <v>86</v>
       </c>
@@ -5896,16 +5896,16 @@
       <c r="E10" s="98">
         <v>76</v>
       </c>
-      <c r="F10" s="140"/>
-      <c r="G10" s="140"/>
-      <c r="H10" s="141"/>
-      <c r="I10" s="141"/>
+      <c r="F10" s="143"/>
+      <c r="G10" s="143"/>
+      <c r="H10" s="144"/>
+      <c r="I10" s="144"/>
       <c r="J10" s="100"/>
       <c r="K10" s="100"/>
       <c r="L10" s="77"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="139"/>
+      <c r="A11" s="142"/>
       <c r="B11" s="99" t="s">
         <v>87</v>
       </c>
@@ -5920,16 +5920,16 @@
       <c r="E11" s="98">
         <v>76</v>
       </c>
-      <c r="F11" s="140"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="141"/>
-      <c r="I11" s="141"/>
+      <c r="F11" s="143"/>
+      <c r="G11" s="143"/>
+      <c r="H11" s="144"/>
+      <c r="I11" s="144"/>
       <c r="J11" s="100"/>
       <c r="K11" s="100"/>
       <c r="L11" s="77"/>
     </row>
     <row r="12" spans="1:12" ht="10.5" customHeight="1">
-      <c r="A12" s="142">
+      <c r="A12" s="139">
         <f>A7+7</f>
         <v>43699</v>
       </c>
@@ -5947,19 +5947,19 @@
       <c r="E12" s="102">
         <v>76</v>
       </c>
-      <c r="F12" s="143">
+      <c r="F12" s="146">
         <f>SUM(E12:E16)</f>
         <v>380</v>
       </c>
-      <c r="G12" s="143">
+      <c r="G12" s="146">
         <f>G7+F12</f>
         <v>608</v>
       </c>
-      <c r="H12" s="144">
+      <c r="H12" s="141">
         <f>F12*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I12" s="144">
+      <c r="I12" s="141">
         <f>I7+H12</f>
         <v>273.60000000000002</v>
       </c>
@@ -5968,7 +5968,7 @@
       <c r="L12" s="77"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="142"/>
+      <c r="A13" s="139"/>
       <c r="B13" s="101" t="s">
         <v>84</v>
       </c>
@@ -5983,16 +5983,16 @@
       <c r="E13" s="102">
         <v>76</v>
       </c>
-      <c r="F13" s="143"/>
-      <c r="G13" s="143"/>
-      <c r="H13" s="144"/>
-      <c r="I13" s="144"/>
+      <c r="F13" s="146"/>
+      <c r="G13" s="146"/>
+      <c r="H13" s="141"/>
+      <c r="I13" s="141"/>
       <c r="J13" s="103"/>
       <c r="K13" s="103"/>
       <c r="L13" s="77"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="142"/>
+      <c r="A14" s="139"/>
       <c r="B14" s="101" t="s">
         <v>85</v>
       </c>
@@ -6007,16 +6007,16 @@
       <c r="E14" s="102">
         <v>76</v>
       </c>
-      <c r="F14" s="143"/>
-      <c r="G14" s="143"/>
-      <c r="H14" s="144"/>
-      <c r="I14" s="144"/>
+      <c r="F14" s="146"/>
+      <c r="G14" s="146"/>
+      <c r="H14" s="141"/>
+      <c r="I14" s="141"/>
       <c r="J14" s="103"/>
       <c r="K14" s="103"/>
       <c r="L14" s="77"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="142"/>
+      <c r="A15" s="139"/>
       <c r="B15" s="101" t="s">
         <v>86</v>
       </c>
@@ -6031,16 +6031,16 @@
       <c r="E15" s="102">
         <v>76</v>
       </c>
-      <c r="F15" s="143"/>
-      <c r="G15" s="143"/>
-      <c r="H15" s="144"/>
-      <c r="I15" s="144"/>
+      <c r="F15" s="146"/>
+      <c r="G15" s="146"/>
+      <c r="H15" s="141"/>
+      <c r="I15" s="141"/>
       <c r="J15" s="103"/>
       <c r="K15" s="103"/>
       <c r="L15" s="77"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="142"/>
+      <c r="A16" s="139"/>
       <c r="B16" s="101" t="s">
         <v>87</v>
       </c>
@@ -6055,16 +6055,16 @@
       <c r="E16" s="102">
         <v>76</v>
       </c>
-      <c r="F16" s="143"/>
-      <c r="G16" s="143"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
+      <c r="F16" s="146"/>
+      <c r="G16" s="146"/>
+      <c r="H16" s="141"/>
+      <c r="I16" s="141"/>
       <c r="J16" s="103"/>
       <c r="K16" s="103"/>
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="139">
+      <c r="A17" s="142">
         <f>A12+7</f>
         <v>43706</v>
       </c>
@@ -6074,19 +6074,19 @@
       <c r="C17" s="98"/>
       <c r="D17" s="98"/>
       <c r="E17" s="98"/>
-      <c r="F17" s="140">
+      <c r="F17" s="143">
         <f>SUM(E17:E21)</f>
         <v>304</v>
       </c>
-      <c r="G17" s="140">
+      <c r="G17" s="143">
         <f>G12+F17</f>
         <v>912</v>
       </c>
-      <c r="H17" s="141">
+      <c r="H17" s="144">
         <f>F17*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I17" s="141">
+      <c r="I17" s="144">
         <f>I12+H17</f>
         <v>410.40000000000003</v>
       </c>
@@ -6095,7 +6095,7 @@
       <c r="L17" s="77"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="139"/>
+      <c r="A18" s="142"/>
       <c r="B18" s="99" t="s">
         <v>84</v>
       </c>
@@ -6110,16 +6110,16 @@
       <c r="E18" s="98">
         <v>76</v>
       </c>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="141"/>
-      <c r="I18" s="141"/>
+      <c r="F18" s="143"/>
+      <c r="G18" s="143"/>
+      <c r="H18" s="144"/>
+      <c r="I18" s="144"/>
       <c r="J18" s="100"/>
       <c r="K18" s="100"/>
       <c r="L18" s="77"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="139"/>
+      <c r="A19" s="142"/>
       <c r="B19" s="99" t="s">
         <v>85</v>
       </c>
@@ -6134,16 +6134,16 @@
       <c r="E19" s="98">
         <v>76</v>
       </c>
-      <c r="F19" s="140"/>
-      <c r="G19" s="140"/>
-      <c r="H19" s="141"/>
-      <c r="I19" s="141"/>
+      <c r="F19" s="143"/>
+      <c r="G19" s="143"/>
+      <c r="H19" s="144"/>
+      <c r="I19" s="144"/>
       <c r="J19" s="100"/>
       <c r="K19" s="100"/>
       <c r="L19" s="77"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="139"/>
+      <c r="A20" s="142"/>
       <c r="B20" s="99" t="s">
         <v>86</v>
       </c>
@@ -6158,16 +6158,16 @@
       <c r="E20" s="98">
         <v>76</v>
       </c>
-      <c r="F20" s="140"/>
-      <c r="G20" s="140"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="141"/>
+      <c r="F20" s="143"/>
+      <c r="G20" s="143"/>
+      <c r="H20" s="144"/>
+      <c r="I20" s="144"/>
       <c r="J20" s="100"/>
       <c r="K20" s="100"/>
       <c r="L20" s="77"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="139"/>
+      <c r="A21" s="142"/>
       <c r="B21" s="99" t="s">
         <v>87</v>
       </c>
@@ -6182,16 +6182,16 @@
       <c r="E21" s="98">
         <v>76</v>
       </c>
-      <c r="F21" s="140"/>
-      <c r="G21" s="140"/>
-      <c r="H21" s="141"/>
-      <c r="I21" s="141"/>
+      <c r="F21" s="143"/>
+      <c r="G21" s="143"/>
+      <c r="H21" s="144"/>
+      <c r="I21" s="144"/>
       <c r="J21" s="100"/>
       <c r="K21" s="100"/>
       <c r="L21" s="77"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="142">
+      <c r="A22" s="139">
         <f>A17+7</f>
         <v>43713</v>
       </c>
@@ -6209,19 +6209,19 @@
       <c r="E22" s="102">
         <v>76</v>
       </c>
-      <c r="F22" s="143">
+      <c r="F22" s="146">
         <f>SUM(E22:E26)</f>
         <v>380</v>
       </c>
-      <c r="G22" s="143">
+      <c r="G22" s="146">
         <f>G17+F22</f>
         <v>1292</v>
       </c>
-      <c r="H22" s="144">
+      <c r="H22" s="141">
         <f>F22*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I22" s="144">
+      <c r="I22" s="141">
         <f>I17+H22</f>
         <v>581.40000000000009</v>
       </c>
@@ -6230,7 +6230,7 @@
       <c r="L22" s="11"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="142"/>
+      <c r="A23" s="139"/>
       <c r="B23" s="101" t="s">
         <v>84</v>
       </c>
@@ -6245,16 +6245,16 @@
       <c r="E23" s="102">
         <v>76</v>
       </c>
-      <c r="F23" s="143"/>
-      <c r="G23" s="143"/>
-      <c r="H23" s="144"/>
-      <c r="I23" s="144"/>
+      <c r="F23" s="146"/>
+      <c r="G23" s="146"/>
+      <c r="H23" s="141"/>
+      <c r="I23" s="141"/>
       <c r="J23" s="103"/>
       <c r="K23" s="103"/>
       <c r="L23" s="77"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="142"/>
+      <c r="A24" s="139"/>
       <c r="B24" s="101" t="s">
         <v>85</v>
       </c>
@@ -6269,16 +6269,16 @@
       <c r="E24" s="102">
         <v>76</v>
       </c>
-      <c r="F24" s="143"/>
-      <c r="G24" s="143"/>
-      <c r="H24" s="144"/>
-      <c r="I24" s="144"/>
+      <c r="F24" s="146"/>
+      <c r="G24" s="146"/>
+      <c r="H24" s="141"/>
+      <c r="I24" s="141"/>
       <c r="J24" s="103"/>
       <c r="K24" s="103"/>
       <c r="L24" s="77"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="142"/>
+      <c r="A25" s="139"/>
       <c r="B25" s="101" t="s">
         <v>86</v>
       </c>
@@ -6293,16 +6293,16 @@
       <c r="E25" s="102">
         <v>76</v>
       </c>
-      <c r="F25" s="143"/>
-      <c r="G25" s="143"/>
-      <c r="H25" s="144"/>
-      <c r="I25" s="144"/>
+      <c r="F25" s="146"/>
+      <c r="G25" s="146"/>
+      <c r="H25" s="141"/>
+      <c r="I25" s="141"/>
       <c r="J25" s="103"/>
       <c r="K25" s="103"/>
       <c r="L25" s="77"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="142"/>
+      <c r="A26" s="139"/>
       <c r="B26" s="101" t="s">
         <v>87</v>
       </c>
@@ -6317,16 +6317,16 @@
       <c r="E26" s="102">
         <v>76</v>
       </c>
-      <c r="F26" s="143"/>
-      <c r="G26" s="143"/>
-      <c r="H26" s="144"/>
-      <c r="I26" s="144"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
+      <c r="H26" s="141"/>
+      <c r="I26" s="141"/>
       <c r="J26" s="103"/>
       <c r="K26" s="103"/>
       <c r="L26" s="77"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="139">
+      <c r="A27" s="142">
         <f>A22+7</f>
         <v>43720</v>
       </c>
@@ -6344,19 +6344,19 @@
       <c r="E27" s="98">
         <v>76</v>
       </c>
-      <c r="F27" s="140">
+      <c r="F27" s="143">
         <f>SUM(E27:E31)</f>
         <v>380</v>
       </c>
-      <c r="G27" s="140">
+      <c r="G27" s="143">
         <f>G22+F27</f>
         <v>1672</v>
       </c>
-      <c r="H27" s="141">
+      <c r="H27" s="144">
         <f>F27*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I27" s="141">
+      <c r="I27" s="144">
         <f>I22+H27</f>
         <v>752.40000000000009</v>
       </c>
@@ -6365,7 +6365,7 @@
       <c r="L27" s="77"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="139"/>
+      <c r="A28" s="142"/>
       <c r="B28" s="99" t="s">
         <v>84</v>
       </c>
@@ -6380,16 +6380,16 @@
       <c r="E28" s="98">
         <v>76</v>
       </c>
-      <c r="F28" s="140"/>
-      <c r="G28" s="140"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="141"/>
+      <c r="F28" s="143"/>
+      <c r="G28" s="143"/>
+      <c r="H28" s="144"/>
+      <c r="I28" s="144"/>
       <c r="J28" s="100"/>
       <c r="K28" s="100"/>
       <c r="L28" s="77"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="139"/>
+      <c r="A29" s="142"/>
       <c r="B29" s="99" t="s">
         <v>85</v>
       </c>
@@ -6404,16 +6404,16 @@
       <c r="E29" s="98">
         <v>76</v>
       </c>
-      <c r="F29" s="140"/>
-      <c r="G29" s="140"/>
-      <c r="H29" s="141"/>
-      <c r="I29" s="141"/>
+      <c r="F29" s="143"/>
+      <c r="G29" s="143"/>
+      <c r="H29" s="144"/>
+      <c r="I29" s="144"/>
       <c r="J29" s="100"/>
       <c r="K29" s="100"/>
       <c r="L29" s="77"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="139"/>
+      <c r="A30" s="142"/>
       <c r="B30" s="99" t="s">
         <v>86</v>
       </c>
@@ -6428,16 +6428,16 @@
       <c r="E30" s="98">
         <v>76</v>
       </c>
-      <c r="F30" s="140"/>
-      <c r="G30" s="140"/>
-      <c r="H30" s="141"/>
-      <c r="I30" s="141"/>
+      <c r="F30" s="143"/>
+      <c r="G30" s="143"/>
+      <c r="H30" s="144"/>
+      <c r="I30" s="144"/>
       <c r="J30" s="100"/>
       <c r="K30" s="100"/>
       <c r="L30" s="77"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="139"/>
+      <c r="A31" s="142"/>
       <c r="B31" s="99" t="s">
         <v>87</v>
       </c>
@@ -6452,16 +6452,16 @@
       <c r="E31" s="98">
         <v>76</v>
       </c>
-      <c r="F31" s="140"/>
-      <c r="G31" s="140"/>
-      <c r="H31" s="141"/>
-      <c r="I31" s="141"/>
+      <c r="F31" s="143"/>
+      <c r="G31" s="143"/>
+      <c r="H31" s="144"/>
+      <c r="I31" s="144"/>
       <c r="J31" s="100"/>
       <c r="K31" s="100"/>
       <c r="L31" s="77"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="142">
+      <c r="A32" s="139">
         <f>A27+7</f>
         <v>43727</v>
       </c>
@@ -6473,19 +6473,19 @@
       <c r="E32" s="102">
         <v>0</v>
       </c>
-      <c r="F32" s="145">
+      <c r="F32" s="140">
         <f>SUM(E32:E36)</f>
         <v>304</v>
       </c>
-      <c r="G32" s="145">
+      <c r="G32" s="140">
         <f>G27+F32</f>
         <v>1976</v>
       </c>
-      <c r="H32" s="144">
+      <c r="H32" s="141">
         <f>F32*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I32" s="144">
+      <c r="I32" s="141">
         <f>I27+H32</f>
         <v>889.2</v>
       </c>
@@ -6496,7 +6496,7 @@
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="142"/>
+      <c r="A33" s="139"/>
       <c r="B33" s="101" t="s">
         <v>84</v>
       </c>
@@ -6511,15 +6511,15 @@
       <c r="E33" s="102">
         <v>76</v>
       </c>
-      <c r="F33" s="145"/>
-      <c r="G33" s="145"/>
-      <c r="H33" s="144"/>
-      <c r="I33" s="144"/>
+      <c r="F33" s="140"/>
+      <c r="G33" s="140"/>
+      <c r="H33" s="141"/>
+      <c r="I33" s="141"/>
       <c r="J33" s="103"/>
       <c r="K33" s="103"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="142"/>
+      <c r="A34" s="139"/>
       <c r="B34" s="101" t="s">
         <v>85</v>
       </c>
@@ -6534,15 +6534,15 @@
       <c r="E34" s="102">
         <v>76</v>
       </c>
-      <c r="F34" s="145"/>
-      <c r="G34" s="145"/>
-      <c r="H34" s="144"/>
-      <c r="I34" s="144"/>
+      <c r="F34" s="140"/>
+      <c r="G34" s="140"/>
+      <c r="H34" s="141"/>
+      <c r="I34" s="141"/>
       <c r="J34" s="103"/>
       <c r="K34" s="103"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="142"/>
+      <c r="A35" s="139"/>
       <c r="B35" s="101" t="s">
         <v>86</v>
       </c>
@@ -6557,15 +6557,15 @@
       <c r="E35" s="102">
         <v>76</v>
       </c>
-      <c r="F35" s="145"/>
-      <c r="G35" s="145"/>
-      <c r="H35" s="144"/>
-      <c r="I35" s="144"/>
+      <c r="F35" s="140"/>
+      <c r="G35" s="140"/>
+      <c r="H35" s="141"/>
+      <c r="I35" s="141"/>
       <c r="J35" s="103"/>
       <c r="K35" s="103"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="142"/>
+      <c r="A36" s="139"/>
       <c r="B36" s="101" t="s">
         <v>87</v>
       </c>
@@ -6580,15 +6580,15 @@
       <c r="E36" s="102">
         <v>76</v>
       </c>
-      <c r="F36" s="145"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="144"/>
-      <c r="I36" s="144"/>
+      <c r="F36" s="140"/>
+      <c r="G36" s="140"/>
+      <c r="H36" s="141"/>
+      <c r="I36" s="141"/>
       <c r="J36" s="103"/>
       <c r="K36" s="103"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="139">
+      <c r="A37" s="142">
         <f>A32+7</f>
         <v>43734</v>
       </c>
@@ -6606,19 +6606,19 @@
       <c r="E37" s="98">
         <v>76</v>
       </c>
-      <c r="F37" s="140">
+      <c r="F37" s="143">
         <f>SUM(E37:E41)</f>
         <v>380</v>
       </c>
-      <c r="G37" s="140">
+      <c r="G37" s="143">
         <f>G32+F37</f>
         <v>2356</v>
       </c>
-      <c r="H37" s="141">
+      <c r="H37" s="144">
         <f>F37*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I37" s="141">
+      <c r="I37" s="144">
         <f>I32+H37</f>
         <v>1060.2</v>
       </c>
@@ -6626,7 +6626,7 @@
       <c r="K37" s="100"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="139"/>
+      <c r="A38" s="142"/>
       <c r="B38" s="99" t="s">
         <v>84</v>
       </c>
@@ -6641,15 +6641,15 @@
       <c r="E38" s="98">
         <v>76</v>
       </c>
-      <c r="F38" s="140"/>
-      <c r="G38" s="140"/>
-      <c r="H38" s="141"/>
-      <c r="I38" s="141"/>
+      <c r="F38" s="143"/>
+      <c r="G38" s="143"/>
+      <c r="H38" s="144"/>
+      <c r="I38" s="144"/>
       <c r="J38" s="100"/>
       <c r="K38" s="100"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="139"/>
+      <c r="A39" s="142"/>
       <c r="B39" s="99" t="s">
         <v>85</v>
       </c>
@@ -6664,15 +6664,15 @@
       <c r="E39" s="98">
         <v>76</v>
       </c>
-      <c r="F39" s="140"/>
-      <c r="G39" s="140"/>
-      <c r="H39" s="141"/>
-      <c r="I39" s="141"/>
+      <c r="F39" s="143"/>
+      <c r="G39" s="143"/>
+      <c r="H39" s="144"/>
+      <c r="I39" s="144"/>
       <c r="J39" s="100"/>
       <c r="K39" s="100"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="139"/>
+      <c r="A40" s="142"/>
       <c r="B40" s="99" t="s">
         <v>86</v>
       </c>
@@ -6687,15 +6687,15 @@
       <c r="E40" s="98">
         <v>76</v>
       </c>
-      <c r="F40" s="140"/>
-      <c r="G40" s="140"/>
-      <c r="H40" s="141"/>
-      <c r="I40" s="141"/>
+      <c r="F40" s="143"/>
+      <c r="G40" s="143"/>
+      <c r="H40" s="144"/>
+      <c r="I40" s="144"/>
       <c r="J40" s="100"/>
       <c r="K40" s="100"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="139"/>
+      <c r="A41" s="142"/>
       <c r="B41" s="99" t="s">
         <v>87</v>
       </c>
@@ -6710,15 +6710,15 @@
       <c r="E41" s="98">
         <v>76</v>
       </c>
-      <c r="F41" s="140"/>
-      <c r="G41" s="140"/>
-      <c r="H41" s="141"/>
-      <c r="I41" s="141"/>
+      <c r="F41" s="143"/>
+      <c r="G41" s="143"/>
+      <c r="H41" s="144"/>
+      <c r="I41" s="144"/>
       <c r="J41" s="100"/>
       <c r="K41" s="100"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="142">
+      <c r="A42" s="139">
         <f>A37+7</f>
         <v>43741</v>
       </c>
@@ -6736,19 +6736,19 @@
       <c r="E42" s="102">
         <v>76</v>
       </c>
-      <c r="F42" s="145">
+      <c r="F42" s="140">
         <f>SUM(E42:E46)</f>
         <v>304</v>
       </c>
-      <c r="G42" s="145">
+      <c r="G42" s="140">
         <f>G37+F42</f>
         <v>2660</v>
       </c>
-      <c r="H42" s="144">
+      <c r="H42" s="141">
         <f>F42*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I42" s="144">
+      <c r="I42" s="141">
         <f>I37+H42</f>
         <v>1197</v>
       </c>
@@ -6756,7 +6756,7 @@
       <c r="K42" s="103"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="142"/>
+      <c r="A43" s="139"/>
       <c r="B43" s="101" t="s">
         <v>84</v>
       </c>
@@ -6771,15 +6771,15 @@
       <c r="E43" s="102">
         <v>76</v>
       </c>
-      <c r="F43" s="145"/>
-      <c r="G43" s="145"/>
-      <c r="H43" s="144"/>
-      <c r="I43" s="144"/>
+      <c r="F43" s="140"/>
+      <c r="G43" s="140"/>
+      <c r="H43" s="141"/>
+      <c r="I43" s="141"/>
       <c r="J43" s="103"/>
       <c r="K43" s="103"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="142"/>
+      <c r="A44" s="139"/>
       <c r="B44" s="101" t="s">
         <v>85</v>
       </c>
@@ -6794,15 +6794,15 @@
       <c r="E44" s="102">
         <v>76</v>
       </c>
-      <c r="F44" s="145"/>
-      <c r="G44" s="145"/>
-      <c r="H44" s="144"/>
-      <c r="I44" s="144"/>
+      <c r="F44" s="140"/>
+      <c r="G44" s="140"/>
+      <c r="H44" s="141"/>
+      <c r="I44" s="141"/>
       <c r="J44" s="103"/>
       <c r="K44" s="103"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="142"/>
+      <c r="A45" s="139"/>
       <c r="B45" s="101" t="s">
         <v>86</v>
       </c>
@@ -6817,15 +6817,15 @@
       <c r="E45" s="102">
         <v>76</v>
       </c>
-      <c r="F45" s="145"/>
-      <c r="G45" s="145"/>
-      <c r="H45" s="144"/>
-      <c r="I45" s="144"/>
+      <c r="F45" s="140"/>
+      <c r="G45" s="140"/>
+      <c r="H45" s="141"/>
+      <c r="I45" s="141"/>
       <c r="J45" s="103"/>
       <c r="K45" s="103"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="142"/>
+      <c r="A46" s="139"/>
       <c r="B46" s="101" t="s">
         <v>87</v>
       </c>
@@ -6834,10 +6834,10 @@
       <c r="E46" s="102">
         <v>0</v>
       </c>
-      <c r="F46" s="145"/>
-      <c r="G46" s="145"/>
-      <c r="H46" s="144"/>
-      <c r="I46" s="144"/>
+      <c r="F46" s="140"/>
+      <c r="G46" s="140"/>
+      <c r="H46" s="141"/>
+      <c r="I46" s="141"/>
       <c r="J46" s="103"/>
       <c r="K46" s="103"/>
       <c r="L46" s="123" t="s">
@@ -6845,7 +6845,7 @@
       </c>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="139">
+      <c r="A47" s="142">
         <f>A42+7</f>
         <v>43748</v>
       </c>
@@ -6857,19 +6857,19 @@
       <c r="E47" s="98">
         <v>0</v>
       </c>
-      <c r="F47" s="140">
+      <c r="F47" s="143">
         <f>SUM(E47:E51)</f>
         <v>304</v>
       </c>
-      <c r="G47" s="140">
+      <c r="G47" s="143">
         <f>G42+F47</f>
         <v>2964</v>
       </c>
-      <c r="H47" s="141">
+      <c r="H47" s="144">
         <f>F47*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I47" s="141">
+      <c r="I47" s="144">
         <f>I42+H47</f>
         <v>1333.8</v>
       </c>
@@ -6880,7 +6880,7 @@
       </c>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="139"/>
+      <c r="A48" s="142"/>
       <c r="B48" s="99" t="s">
         <v>84</v>
       </c>
@@ -6895,15 +6895,15 @@
       <c r="E48" s="98">
         <v>76</v>
       </c>
-      <c r="F48" s="140"/>
-      <c r="G48" s="140"/>
-      <c r="H48" s="141"/>
-      <c r="I48" s="141"/>
+      <c r="F48" s="143"/>
+      <c r="G48" s="143"/>
+      <c r="H48" s="144"/>
+      <c r="I48" s="144"/>
       <c r="J48" s="100"/>
       <c r="K48" s="100"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="139"/>
+      <c r="A49" s="142"/>
       <c r="B49" s="99" t="s">
         <v>85</v>
       </c>
@@ -6918,15 +6918,15 @@
       <c r="E49" s="98">
         <v>76</v>
       </c>
-      <c r="F49" s="140"/>
-      <c r="G49" s="140"/>
-      <c r="H49" s="141"/>
-      <c r="I49" s="141"/>
+      <c r="F49" s="143"/>
+      <c r="G49" s="143"/>
+      <c r="H49" s="144"/>
+      <c r="I49" s="144"/>
       <c r="J49" s="100"/>
       <c r="K49" s="100"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="139"/>
+      <c r="A50" s="142"/>
       <c r="B50" s="99" t="s">
         <v>86</v>
       </c>
@@ -6941,15 +6941,15 @@
       <c r="E50" s="98">
         <v>76</v>
       </c>
-      <c r="F50" s="140"/>
-      <c r="G50" s="140"/>
-      <c r="H50" s="141"/>
-      <c r="I50" s="141"/>
+      <c r="F50" s="143"/>
+      <c r="G50" s="143"/>
+      <c r="H50" s="144"/>
+      <c r="I50" s="144"/>
       <c r="J50" s="100"/>
       <c r="K50" s="100"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="139"/>
+      <c r="A51" s="142"/>
       <c r="B51" s="99" t="s">
         <v>87</v>
       </c>
@@ -6964,32 +6964,32 @@
       <c r="E51" s="98">
         <v>76</v>
       </c>
-      <c r="F51" s="140"/>
-      <c r="G51" s="140"/>
-      <c r="H51" s="141"/>
-      <c r="I51" s="141"/>
+      <c r="F51" s="143"/>
+      <c r="G51" s="143"/>
+      <c r="H51" s="144"/>
+      <c r="I51" s="144"/>
       <c r="J51" s="100"/>
       <c r="K51" s="100"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="142"/>
+      <c r="A52" s="139"/>
       <c r="B52" s="101"/>
       <c r="C52" s="102"/>
       <c r="D52" s="102"/>
       <c r="E52" s="102"/>
-      <c r="F52" s="145">
+      <c r="F52" s="140">
         <f>SUM(E52:E56)</f>
         <v>0</v>
       </c>
-      <c r="G52" s="145">
+      <c r="G52" s="140">
         <f>G47+F52</f>
         <v>2964</v>
       </c>
-      <c r="H52" s="144">
+      <c r="H52" s="141">
         <f>F52*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I52" s="144">
+      <c r="I52" s="141">
         <f>I47+H52</f>
         <v>1333.8</v>
       </c>
@@ -6997,76 +6997,76 @@
       <c r="K52" s="103"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="142"/>
+      <c r="A53" s="139"/>
       <c r="B53" s="101"/>
       <c r="C53" s="102"/>
       <c r="D53" s="102"/>
       <c r="E53" s="102"/>
-      <c r="F53" s="145"/>
-      <c r="G53" s="145"/>
-      <c r="H53" s="144"/>
-      <c r="I53" s="144"/>
+      <c r="F53" s="140"/>
+      <c r="G53" s="140"/>
+      <c r="H53" s="141"/>
+      <c r="I53" s="141"/>
       <c r="J53" s="103"/>
       <c r="K53" s="103"/>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="142"/>
+      <c r="A54" s="139"/>
       <c r="B54" s="101"/>
       <c r="C54" s="102"/>
       <c r="D54" s="102"/>
       <c r="E54" s="102"/>
-      <c r="F54" s="145"/>
-      <c r="G54" s="145"/>
-      <c r="H54" s="144"/>
-      <c r="I54" s="144"/>
+      <c r="F54" s="140"/>
+      <c r="G54" s="140"/>
+      <c r="H54" s="141"/>
+      <c r="I54" s="141"/>
       <c r="J54" s="103"/>
       <c r="K54" s="103"/>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="142"/>
+      <c r="A55" s="139"/>
       <c r="B55" s="101"/>
       <c r="C55" s="102"/>
       <c r="D55" s="102"/>
       <c r="E55" s="102"/>
-      <c r="F55" s="145"/>
-      <c r="G55" s="145"/>
-      <c r="H55" s="144"/>
-      <c r="I55" s="144"/>
+      <c r="F55" s="140"/>
+      <c r="G55" s="140"/>
+      <c r="H55" s="141"/>
+      <c r="I55" s="141"/>
       <c r="J55" s="103"/>
       <c r="K55" s="103"/>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="142"/>
+      <c r="A56" s="139"/>
       <c r="B56" s="101"/>
       <c r="C56" s="102"/>
       <c r="D56" s="102"/>
       <c r="E56" s="102"/>
-      <c r="F56" s="145"/>
-      <c r="G56" s="145"/>
-      <c r="H56" s="144"/>
-      <c r="I56" s="144"/>
+      <c r="F56" s="140"/>
+      <c r="G56" s="140"/>
+      <c r="H56" s="141"/>
+      <c r="I56" s="141"/>
       <c r="J56" s="103"/>
       <c r="K56" s="103"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="139"/>
+      <c r="A57" s="142"/>
       <c r="B57" s="99"/>
       <c r="C57" s="98"/>
       <c r="D57" s="98"/>
       <c r="E57" s="98"/>
-      <c r="F57" s="140">
+      <c r="F57" s="143">
         <f>SUM(E57:E61)</f>
         <v>0</v>
       </c>
-      <c r="G57" s="140">
+      <c r="G57" s="143">
         <f>G52+F57</f>
         <v>2964</v>
       </c>
-      <c r="H57" s="141">
+      <c r="H57" s="144">
         <f>F57*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I57" s="141">
+      <c r="I57" s="144">
         <f>I52+H57</f>
         <v>1333.8</v>
       </c>
@@ -7074,76 +7074,76 @@
       <c r="K57" s="100"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="139"/>
+      <c r="A58" s="142"/>
       <c r="B58" s="99"/>
       <c r="C58" s="98"/>
       <c r="D58" s="98"/>
       <c r="E58" s="98"/>
-      <c r="F58" s="140"/>
-      <c r="G58" s="140"/>
-      <c r="H58" s="141"/>
-      <c r="I58" s="141"/>
+      <c r="F58" s="143"/>
+      <c r="G58" s="143"/>
+      <c r="H58" s="144"/>
+      <c r="I58" s="144"/>
       <c r="J58" s="100"/>
       <c r="K58" s="100"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="139"/>
+      <c r="A59" s="142"/>
       <c r="B59" s="99"/>
       <c r="C59" s="98"/>
       <c r="D59" s="98"/>
       <c r="E59" s="98"/>
-      <c r="F59" s="140"/>
-      <c r="G59" s="140"/>
-      <c r="H59" s="141"/>
-      <c r="I59" s="141"/>
+      <c r="F59" s="143"/>
+      <c r="G59" s="143"/>
+      <c r="H59" s="144"/>
+      <c r="I59" s="144"/>
       <c r="J59" s="100"/>
       <c r="K59" s="100"/>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="139"/>
+      <c r="A60" s="142"/>
       <c r="B60" s="99"/>
       <c r="C60" s="98"/>
       <c r="D60" s="98"/>
       <c r="E60" s="98"/>
-      <c r="F60" s="140"/>
-      <c r="G60" s="140"/>
-      <c r="H60" s="141"/>
-      <c r="I60" s="141"/>
+      <c r="F60" s="143"/>
+      <c r="G60" s="143"/>
+      <c r="H60" s="144"/>
+      <c r="I60" s="144"/>
       <c r="J60" s="100"/>
       <c r="K60" s="100"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="139"/>
+      <c r="A61" s="142"/>
       <c r="B61" s="99"/>
       <c r="C61" s="98"/>
       <c r="D61" s="98"/>
       <c r="E61" s="98"/>
-      <c r="F61" s="140"/>
-      <c r="G61" s="140"/>
-      <c r="H61" s="141"/>
-      <c r="I61" s="141"/>
+      <c r="F61" s="143"/>
+      <c r="G61" s="143"/>
+      <c r="H61" s="144"/>
+      <c r="I61" s="144"/>
       <c r="J61" s="100"/>
       <c r="K61" s="100"/>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="142"/>
+      <c r="A62" s="139"/>
       <c r="B62" s="101"/>
       <c r="C62" s="102"/>
       <c r="D62" s="102"/>
       <c r="E62" s="102"/>
-      <c r="F62" s="145">
+      <c r="F62" s="140">
         <f>SUM(E62:E66)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="145">
+      <c r="G62" s="140">
         <f>G57+F62</f>
         <v>2964</v>
       </c>
-      <c r="H62" s="144">
+      <c r="H62" s="141">
         <f>F62*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I62" s="144">
+      <c r="I62" s="141">
         <f>I57+H62</f>
         <v>1333.8</v>
       </c>
@@ -7151,120 +7151,120 @@
       <c r="K62" s="103"/>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="142"/>
+      <c r="A63" s="139"/>
       <c r="B63" s="101"/>
       <c r="C63" s="102"/>
       <c r="D63" s="102"/>
       <c r="E63" s="102"/>
-      <c r="F63" s="145"/>
-      <c r="G63" s="145"/>
-      <c r="H63" s="144"/>
-      <c r="I63" s="144"/>
+      <c r="F63" s="140"/>
+      <c r="G63" s="140"/>
+      <c r="H63" s="141"/>
+      <c r="I63" s="141"/>
       <c r="J63" s="103"/>
       <c r="K63" s="103"/>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="142"/>
+      <c r="A64" s="139"/>
       <c r="B64" s="101"/>
       <c r="C64" s="102"/>
       <c r="D64" s="102"/>
       <c r="E64" s="102"/>
-      <c r="F64" s="145"/>
-      <c r="G64" s="145"/>
-      <c r="H64" s="144"/>
-      <c r="I64" s="144"/>
+      <c r="F64" s="140"/>
+      <c r="G64" s="140"/>
+      <c r="H64" s="141"/>
+      <c r="I64" s="141"/>
       <c r="J64" s="103"/>
       <c r="K64" s="103"/>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="142"/>
+      <c r="A65" s="139"/>
       <c r="B65" s="101"/>
       <c r="C65" s="102"/>
       <c r="D65" s="102"/>
       <c r="E65" s="102"/>
-      <c r="F65" s="145"/>
-      <c r="G65" s="145"/>
-      <c r="H65" s="144"/>
-      <c r="I65" s="144"/>
+      <c r="F65" s="140"/>
+      <c r="G65" s="140"/>
+      <c r="H65" s="141"/>
+      <c r="I65" s="141"/>
       <c r="J65" s="103"/>
       <c r="K65" s="103"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="142"/>
+      <c r="A66" s="139"/>
       <c r="B66" s="101"/>
       <c r="C66" s="102"/>
       <c r="D66" s="102"/>
       <c r="E66" s="102"/>
-      <c r="F66" s="145"/>
-      <c r="G66" s="145"/>
-      <c r="H66" s="144"/>
-      <c r="I66" s="144"/>
+      <c r="F66" s="140"/>
+      <c r="G66" s="140"/>
+      <c r="H66" s="141"/>
+      <c r="I66" s="141"/>
       <c r="J66" s="103"/>
       <c r="K66" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="F62:F66"/>
-    <mergeCell ref="G62:G66"/>
-    <mergeCell ref="H62:H66"/>
-    <mergeCell ref="I62:I66"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="F52:F56"/>
-    <mergeCell ref="G52:G56"/>
-    <mergeCell ref="H52:H56"/>
-    <mergeCell ref="I52:I56"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="F57:F61"/>
-    <mergeCell ref="G57:G61"/>
-    <mergeCell ref="H57:H61"/>
-    <mergeCell ref="I57:I61"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="F37:F41"/>
-    <mergeCell ref="G37:G41"/>
-    <mergeCell ref="H37:H41"/>
-    <mergeCell ref="I37:I41"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="F47:F51"/>
-    <mergeCell ref="G47:G51"/>
-    <mergeCell ref="H47:H51"/>
-    <mergeCell ref="I47:I51"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="F42:F46"/>
-    <mergeCell ref="G42:G46"/>
-    <mergeCell ref="H42:H46"/>
-    <mergeCell ref="I42:I46"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="G27:G31"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="G22:G26"/>
+    <mergeCell ref="H22:H26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="G32:G36"/>
+    <mergeCell ref="H32:H36"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="I17:I21"/>
     <mergeCell ref="I7:I11"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="F12:F16"/>
     <mergeCell ref="G12:G16"/>
     <mergeCell ref="H12:H16"/>
     <mergeCell ref="I12:I16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="F17:F21"/>
-    <mergeCell ref="G17:G21"/>
-    <mergeCell ref="H17:H21"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="F32:F36"/>
-    <mergeCell ref="G32:G36"/>
-    <mergeCell ref="H32:H36"/>
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="G22:G26"/>
-    <mergeCell ref="H22:H26"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="G27:G31"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="F42:F46"/>
+    <mergeCell ref="G42:G46"/>
+    <mergeCell ref="H42:H46"/>
+    <mergeCell ref="I42:I46"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="F47:F51"/>
+    <mergeCell ref="G47:G51"/>
+    <mergeCell ref="H47:H51"/>
+    <mergeCell ref="I47:I51"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="F37:F41"/>
+    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="H37:H41"/>
+    <mergeCell ref="I37:I41"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="F57:F61"/>
+    <mergeCell ref="G57:G61"/>
+    <mergeCell ref="H57:H61"/>
+    <mergeCell ref="I57:I61"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="F52:F56"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="H52:H56"/>
+    <mergeCell ref="I52:I56"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="F62:F66"/>
+    <mergeCell ref="G62:G66"/>
+    <mergeCell ref="H62:H66"/>
+    <mergeCell ref="I62:I66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="portrait"/>

</xml_diff>

<commit_message>
Moved Core test files into new project Lava3.Core.Test
</commit_message>
<xml_diff>
--- a/Lava3.Test/TestFiles/Test.xlsx
+++ b/Lava3.Test/TestFiles/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="585" windowWidth="15555" windowHeight="18030" tabRatio="554" activeTab="2"/>
+    <workbookView xWindow="510" yWindow="585" windowWidth="15555" windowHeight="18030" tabRatio="554" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Annual Summary" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="105">
   <si>
     <t>Description</t>
   </si>
@@ -286,12 +286,6 @@
   </si>
   <si>
     <t>Fri</t>
-  </si>
-  <si>
-    <t>Ill</t>
-  </si>
-  <si>
-    <t>Holiday</t>
   </si>
   <si>
     <t>PluralSight</t>
@@ -1982,7 +1976,7 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="13"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="149">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2194,15 +2188,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2212,11 +2197,24 @@
     <xf numFmtId="44" fontId="20" fillId="0" borderId="0" xfId="763" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="45" fillId="4" borderId="0" xfId="773" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="931">
@@ -3539,7 +3537,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="12.75">
       <c r="A1" s="87" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" s="87"/>
       <c r="D1" s="23"/>
@@ -4909,7 +4907,7 @@
         <v>42609</v>
       </c>
       <c r="B6" s="133" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="127">
         <v>3.1</v>
@@ -4929,7 +4927,7 @@
         <v>42610</v>
       </c>
       <c r="B7" s="127" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="127">
         <v>0</v>
@@ -4969,7 +4967,7 @@
         <v>42612</v>
       </c>
       <c r="B9" s="132" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C9" s="127">
         <v>14.5</v>
@@ -5002,7 +5000,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
@@ -5125,7 +5123,7 @@
         <v>42581</v>
       </c>
       <c r="D5" s="126" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E5" s="61">
         <v>-22.15</v>
@@ -5147,7 +5145,7 @@
         <v>42581</v>
       </c>
       <c r="D6" s="126" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E6" s="61">
         <v>-0.66</v>
@@ -5165,7 +5163,7 @@
         <v>42585</v>
       </c>
       <c r="D7" s="126" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E7" s="61">
         <v>-6.85</v>
@@ -5195,7 +5193,7 @@
         <v>42592</v>
       </c>
       <c r="D9" s="126" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E9" s="61">
         <v>-174</v>
@@ -5208,7 +5206,7 @@
         <v>42593</v>
       </c>
       <c r="D10" s="126" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E10" s="61">
         <v>-35.020000000000003</v>
@@ -5221,7 +5219,7 @@
         <v>42594</v>
       </c>
       <c r="D11" s="126" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E11" s="61">
         <v>-11.99</v>
@@ -5532,7 +5530,7 @@
     </row>
     <row r="18" spans="1:3" s="43" customFormat="1">
       <c r="A18" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B18" s="43" t="s">
         <v>6</v>
@@ -5540,7 +5538,7 @@
     </row>
     <row r="19" spans="1:3" s="67" customFormat="1">
       <c r="A19" s="99" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B19" s="79" t="s">
         <v>8</v>
@@ -5548,7 +5546,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="124" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B20" s="106" t="s">
         <v>7</v>
@@ -5556,7 +5554,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="99" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B21" s="74" t="s">
         <v>9</v>
@@ -5564,7 +5562,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="124" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -5572,7 +5570,7 @@
     </row>
     <row r="23" spans="1:3" s="52" customFormat="1">
       <c r="A23" s="124" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B23" s="52" t="s">
         <v>10</v>
@@ -5602,10 +5600,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="124" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" s="124" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -5625,7 +5623,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B33" s="109" t="s">
         <v>25</v>
@@ -5633,24 +5631,24 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="99" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B34" s="74" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="124" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="99" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B35" s="107" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="124" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -5671,17 +5669,17 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="22.125" customWidth="1"/>
     <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
-    <col min="5" max="5" width="8.875" customWidth="1"/>
+    <col min="3" max="3" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.875" customWidth="1"/>
@@ -5699,11 +5697,11 @@
       <c r="K1" s="51"/>
     </row>
     <row r="2" spans="1:12" s="48" customFormat="1">
-      <c r="E2" s="145" t="s">
+      <c r="E2" s="146" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
       <c r="H2" s="49" t="s">
         <v>72</v>
       </c>
@@ -5753,24 +5751,30 @@
         <v>81</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="60">
-        <f>MIN(C7,C729)</f>
-        <v>0</v>
+      <c r="C4" s="147">
+        <f>SMALL(C7:C100,COUNTIF($C$7:$C$100,0)+1)</f>
+        <v>81000</v>
       </c>
       <c r="D4" s="60">
         <f>MAX(D7:D121)</f>
         <v>83964</v>
       </c>
-      <c r="E4" s="60">
-        <f>AVERAGE(E7:E66,E729)</f>
-        <v>67.36363636363636</v>
-      </c>
-      <c r="F4" s="11"/>
+      <c r="E4" s="148">
+        <f>AVERAGEIF(E7:E1000,"&lt;&gt;0")</f>
+        <v>76</v>
+      </c>
+      <c r="F4" s="148">
+        <f>AVERAGEIF(F7:F1000,"&lt;&gt;0")</f>
+        <v>329.33333333333331</v>
+      </c>
       <c r="G4" s="91">
-        <f>SUM(E7:E273)</f>
+        <f>SUM(E7:E2073)</f>
         <v>2964</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="148">
+        <f>AVERAGEIF(H7:H1000,"&lt;&gt;0")</f>
+        <v>148.19999999999999</v>
+      </c>
       <c r="I4" s="61">
         <f>MAX(I7:I329)</f>
         <v>1333.8</v>
@@ -5808,7 +5812,7 @@
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="142">
+      <c r="A7" s="139">
         <v>43692</v>
       </c>
       <c r="B7" s="99" t="s">
@@ -5819,19 +5823,19 @@
       <c r="E7" s="98">
         <v>0</v>
       </c>
-      <c r="F7" s="143">
+      <c r="F7" s="140">
         <f>SUM(E7:E11)</f>
         <v>228</v>
       </c>
-      <c r="G7" s="143">
+      <c r="G7" s="140">
         <f>F7</f>
         <v>228</v>
       </c>
-      <c r="H7" s="144">
+      <c r="H7" s="141">
         <f>F7*$I$2</f>
         <v>102.60000000000001</v>
       </c>
-      <c r="I7" s="144">
+      <c r="I7" s="141">
         <f>H7</f>
         <v>102.60000000000001</v>
       </c>
@@ -5840,7 +5844,7 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="142"/>
+      <c r="A8" s="139"/>
       <c r="B8" s="99" t="s">
         <v>84</v>
       </c>
@@ -5849,16 +5853,16 @@
       <c r="E8" s="98">
         <v>0</v>
       </c>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="144"/>
-      <c r="I8" s="144"/>
+      <c r="F8" s="140"/>
+      <c r="G8" s="140"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
       <c r="J8" s="100"/>
       <c r="K8" s="100"/>
       <c r="L8" s="77"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="142"/>
+      <c r="A9" s="139"/>
       <c r="B9" s="99" t="s">
         <v>85</v>
       </c>
@@ -5872,16 +5876,16 @@
       <c r="E9" s="98">
         <v>76</v>
       </c>
-      <c r="F9" s="143"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="144"/>
-      <c r="I9" s="144"/>
+      <c r="F9" s="140"/>
+      <c r="G9" s="140"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="141"/>
       <c r="J9" s="100"/>
       <c r="K9" s="100"/>
       <c r="L9" s="77"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="142"/>
+      <c r="A10" s="139"/>
       <c r="B10" s="99" t="s">
         <v>86</v>
       </c>
@@ -5896,16 +5900,16 @@
       <c r="E10" s="98">
         <v>76</v>
       </c>
-      <c r="F10" s="143"/>
-      <c r="G10" s="143"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="144"/>
+      <c r="F10" s="140"/>
+      <c r="G10" s="140"/>
+      <c r="H10" s="141"/>
+      <c r="I10" s="141"/>
       <c r="J10" s="100"/>
       <c r="K10" s="100"/>
       <c r="L10" s="77"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="142"/>
+      <c r="A11" s="139"/>
       <c r="B11" s="99" t="s">
         <v>87</v>
       </c>
@@ -5920,16 +5924,16 @@
       <c r="E11" s="98">
         <v>76</v>
       </c>
-      <c r="F11" s="143"/>
-      <c r="G11" s="143"/>
-      <c r="H11" s="144"/>
-      <c r="I11" s="144"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="141"/>
       <c r="J11" s="100"/>
       <c r="K11" s="100"/>
       <c r="L11" s="77"/>
     </row>
     <row r="12" spans="1:12" ht="10.5" customHeight="1">
-      <c r="A12" s="139">
+      <c r="A12" s="142">
         <f>A7+7</f>
         <v>43699</v>
       </c>
@@ -5947,19 +5951,19 @@
       <c r="E12" s="102">
         <v>76</v>
       </c>
-      <c r="F12" s="146">
+      <c r="F12" s="143">
         <f>SUM(E12:E16)</f>
         <v>380</v>
       </c>
-      <c r="G12" s="146">
+      <c r="G12" s="143">
         <f>G7+F12</f>
         <v>608</v>
       </c>
-      <c r="H12" s="141">
+      <c r="H12" s="144">
         <f>F12*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I12" s="141">
+      <c r="I12" s="144">
         <f>I7+H12</f>
         <v>273.60000000000002</v>
       </c>
@@ -5968,7 +5972,7 @@
       <c r="L12" s="77"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="139"/>
+      <c r="A13" s="142"/>
       <c r="B13" s="101" t="s">
         <v>84</v>
       </c>
@@ -5983,16 +5987,16 @@
       <c r="E13" s="102">
         <v>76</v>
       </c>
-      <c r="F13" s="146"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="141"/>
-      <c r="I13" s="141"/>
+      <c r="F13" s="143"/>
+      <c r="G13" s="143"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="144"/>
       <c r="J13" s="103"/>
       <c r="K13" s="103"/>
       <c r="L13" s="77"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="139"/>
+      <c r="A14" s="142"/>
       <c r="B14" s="101" t="s">
         <v>85</v>
       </c>
@@ -6007,16 +6011,16 @@
       <c r="E14" s="102">
         <v>76</v>
       </c>
-      <c r="F14" s="146"/>
-      <c r="G14" s="146"/>
-      <c r="H14" s="141"/>
-      <c r="I14" s="141"/>
+      <c r="F14" s="143"/>
+      <c r="G14" s="143"/>
+      <c r="H14" s="144"/>
+      <c r="I14" s="144"/>
       <c r="J14" s="103"/>
       <c r="K14" s="103"/>
       <c r="L14" s="77"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="139"/>
+      <c r="A15" s="142"/>
       <c r="B15" s="101" t="s">
         <v>86</v>
       </c>
@@ -6031,16 +6035,16 @@
       <c r="E15" s="102">
         <v>76</v>
       </c>
-      <c r="F15" s="146"/>
-      <c r="G15" s="146"/>
-      <c r="H15" s="141"/>
-      <c r="I15" s="141"/>
+      <c r="F15" s="143"/>
+      <c r="G15" s="143"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="144"/>
       <c r="J15" s="103"/>
       <c r="K15" s="103"/>
       <c r="L15" s="77"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="139"/>
+      <c r="A16" s="142"/>
       <c r="B16" s="101" t="s">
         <v>87</v>
       </c>
@@ -6055,16 +6059,16 @@
       <c r="E16" s="102">
         <v>76</v>
       </c>
-      <c r="F16" s="146"/>
-      <c r="G16" s="146"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="141"/>
+      <c r="F16" s="143"/>
+      <c r="G16" s="143"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
       <c r="J16" s="103"/>
       <c r="K16" s="103"/>
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="142">
+      <c r="A17" s="139">
         <f>A12+7</f>
         <v>43706</v>
       </c>
@@ -6074,19 +6078,19 @@
       <c r="C17" s="98"/>
       <c r="D17" s="98"/>
       <c r="E17" s="98"/>
-      <c r="F17" s="143">
+      <c r="F17" s="140">
         <f>SUM(E17:E21)</f>
         <v>304</v>
       </c>
-      <c r="G17" s="143">
+      <c r="G17" s="140">
         <f>G12+F17</f>
         <v>912</v>
       </c>
-      <c r="H17" s="144">
+      <c r="H17" s="141">
         <f>F17*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I17" s="144">
+      <c r="I17" s="141">
         <f>I12+H17</f>
         <v>410.40000000000003</v>
       </c>
@@ -6095,7 +6099,7 @@
       <c r="L17" s="77"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="142"/>
+      <c r="A18" s="139"/>
       <c r="B18" s="99" t="s">
         <v>84</v>
       </c>
@@ -6110,16 +6114,16 @@
       <c r="E18" s="98">
         <v>76</v>
       </c>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="144"/>
+      <c r="F18" s="140"/>
+      <c r="G18" s="140"/>
+      <c r="H18" s="141"/>
+      <c r="I18" s="141"/>
       <c r="J18" s="100"/>
       <c r="K18" s="100"/>
       <c r="L18" s="77"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="142"/>
+      <c r="A19" s="139"/>
       <c r="B19" s="99" t="s">
         <v>85</v>
       </c>
@@ -6134,16 +6138,16 @@
       <c r="E19" s="98">
         <v>76</v>
       </c>
-      <c r="F19" s="143"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="144"/>
-      <c r="I19" s="144"/>
+      <c r="F19" s="140"/>
+      <c r="G19" s="140"/>
+      <c r="H19" s="141"/>
+      <c r="I19" s="141"/>
       <c r="J19" s="100"/>
       <c r="K19" s="100"/>
       <c r="L19" s="77"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="142"/>
+      <c r="A20" s="139"/>
       <c r="B20" s="99" t="s">
         <v>86</v>
       </c>
@@ -6158,16 +6162,16 @@
       <c r="E20" s="98">
         <v>76</v>
       </c>
-      <c r="F20" s="143"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="144"/>
-      <c r="I20" s="144"/>
+      <c r="F20" s="140"/>
+      <c r="G20" s="140"/>
+      <c r="H20" s="141"/>
+      <c r="I20" s="141"/>
       <c r="J20" s="100"/>
       <c r="K20" s="100"/>
       <c r="L20" s="77"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="142"/>
+      <c r="A21" s="139"/>
       <c r="B21" s="99" t="s">
         <v>87</v>
       </c>
@@ -6182,16 +6186,16 @@
       <c r="E21" s="98">
         <v>76</v>
       </c>
-      <c r="F21" s="143"/>
-      <c r="G21" s="143"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="144"/>
+      <c r="F21" s="140"/>
+      <c r="G21" s="140"/>
+      <c r="H21" s="141"/>
+      <c r="I21" s="141"/>
       <c r="J21" s="100"/>
       <c r="K21" s="100"/>
       <c r="L21" s="77"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="139">
+      <c r="A22" s="142">
         <f>A17+7</f>
         <v>43713</v>
       </c>
@@ -6209,19 +6213,19 @@
       <c r="E22" s="102">
         <v>76</v>
       </c>
-      <c r="F22" s="146">
+      <c r="F22" s="143">
         <f>SUM(E22:E26)</f>
         <v>380</v>
       </c>
-      <c r="G22" s="146">
+      <c r="G22" s="143">
         <f>G17+F22</f>
         <v>1292</v>
       </c>
-      <c r="H22" s="141">
+      <c r="H22" s="144">
         <f>F22*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I22" s="141">
+      <c r="I22" s="144">
         <f>I17+H22</f>
         <v>581.40000000000009</v>
       </c>
@@ -6230,7 +6234,7 @@
       <c r="L22" s="11"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="139"/>
+      <c r="A23" s="142"/>
       <c r="B23" s="101" t="s">
         <v>84</v>
       </c>
@@ -6245,16 +6249,16 @@
       <c r="E23" s="102">
         <v>76</v>
       </c>
-      <c r="F23" s="146"/>
-      <c r="G23" s="146"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="141"/>
+      <c r="F23" s="143"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="144"/>
+      <c r="I23" s="144"/>
       <c r="J23" s="103"/>
       <c r="K23" s="103"/>
       <c r="L23" s="77"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="139"/>
+      <c r="A24" s="142"/>
       <c r="B24" s="101" t="s">
         <v>85</v>
       </c>
@@ -6269,16 +6273,16 @@
       <c r="E24" s="102">
         <v>76</v>
       </c>
-      <c r="F24" s="146"/>
-      <c r="G24" s="146"/>
-      <c r="H24" s="141"/>
-      <c r="I24" s="141"/>
+      <c r="F24" s="143"/>
+      <c r="G24" s="143"/>
+      <c r="H24" s="144"/>
+      <c r="I24" s="144"/>
       <c r="J24" s="103"/>
       <c r="K24" s="103"/>
       <c r="L24" s="77"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="139"/>
+      <c r="A25" s="142"/>
       <c r="B25" s="101" t="s">
         <v>86</v>
       </c>
@@ -6293,16 +6297,16 @@
       <c r="E25" s="102">
         <v>76</v>
       </c>
-      <c r="F25" s="146"/>
-      <c r="G25" s="146"/>
-      <c r="H25" s="141"/>
-      <c r="I25" s="141"/>
+      <c r="F25" s="143"/>
+      <c r="G25" s="143"/>
+      <c r="H25" s="144"/>
+      <c r="I25" s="144"/>
       <c r="J25" s="103"/>
       <c r="K25" s="103"/>
       <c r="L25" s="77"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="139"/>
+      <c r="A26" s="142"/>
       <c r="B26" s="101" t="s">
         <v>87</v>
       </c>
@@ -6317,16 +6321,16 @@
       <c r="E26" s="102">
         <v>76</v>
       </c>
-      <c r="F26" s="146"/>
-      <c r="G26" s="146"/>
-      <c r="H26" s="141"/>
-      <c r="I26" s="141"/>
+      <c r="F26" s="143"/>
+      <c r="G26" s="143"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="144"/>
       <c r="J26" s="103"/>
       <c r="K26" s="103"/>
       <c r="L26" s="77"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="142">
+      <c r="A27" s="139">
         <f>A22+7</f>
         <v>43720</v>
       </c>
@@ -6344,19 +6348,19 @@
       <c r="E27" s="98">
         <v>76</v>
       </c>
-      <c r="F27" s="143">
+      <c r="F27" s="140">
         <f>SUM(E27:E31)</f>
         <v>380</v>
       </c>
-      <c r="G27" s="143">
+      <c r="G27" s="140">
         <f>G22+F27</f>
         <v>1672</v>
       </c>
-      <c r="H27" s="144">
+      <c r="H27" s="141">
         <f>F27*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I27" s="144">
+      <c r="I27" s="141">
         <f>I22+H27</f>
         <v>752.40000000000009</v>
       </c>
@@ -6365,7 +6369,7 @@
       <c r="L27" s="77"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="142"/>
+      <c r="A28" s="139"/>
       <c r="B28" s="99" t="s">
         <v>84</v>
       </c>
@@ -6380,16 +6384,16 @@
       <c r="E28" s="98">
         <v>76</v>
       </c>
-      <c r="F28" s="143"/>
-      <c r="G28" s="143"/>
-      <c r="H28" s="144"/>
-      <c r="I28" s="144"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="141"/>
+      <c r="I28" s="141"/>
       <c r="J28" s="100"/>
       <c r="K28" s="100"/>
       <c r="L28" s="77"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="142"/>
+      <c r="A29" s="139"/>
       <c r="B29" s="99" t="s">
         <v>85</v>
       </c>
@@ -6404,16 +6408,16 @@
       <c r="E29" s="98">
         <v>76</v>
       </c>
-      <c r="F29" s="143"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="144"/>
-      <c r="I29" s="144"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="141"/>
+      <c r="I29" s="141"/>
       <c r="J29" s="100"/>
       <c r="K29" s="100"/>
       <c r="L29" s="77"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="142"/>
+      <c r="A30" s="139"/>
       <c r="B30" s="99" t="s">
         <v>86</v>
       </c>
@@ -6428,16 +6432,16 @@
       <c r="E30" s="98">
         <v>76</v>
       </c>
-      <c r="F30" s="143"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="144"/>
-      <c r="I30" s="144"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="141"/>
+      <c r="I30" s="141"/>
       <c r="J30" s="100"/>
       <c r="K30" s="100"/>
       <c r="L30" s="77"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="142"/>
+      <c r="A31" s="139"/>
       <c r="B31" s="99" t="s">
         <v>87</v>
       </c>
@@ -6452,16 +6456,16 @@
       <c r="E31" s="98">
         <v>76</v>
       </c>
-      <c r="F31" s="143"/>
-      <c r="G31" s="143"/>
-      <c r="H31" s="144"/>
-      <c r="I31" s="144"/>
+      <c r="F31" s="140"/>
+      <c r="G31" s="140"/>
+      <c r="H31" s="141"/>
+      <c r="I31" s="141"/>
       <c r="J31" s="100"/>
       <c r="K31" s="100"/>
       <c r="L31" s="77"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="139">
+      <c r="A32" s="142">
         <f>A27+7</f>
         <v>43727</v>
       </c>
@@ -6473,30 +6477,28 @@
       <c r="E32" s="102">
         <v>0</v>
       </c>
-      <c r="F32" s="140">
+      <c r="F32" s="145">
         <f>SUM(E32:E36)</f>
         <v>304</v>
       </c>
-      <c r="G32" s="140">
+      <c r="G32" s="145">
         <f>G27+F32</f>
         <v>1976</v>
       </c>
-      <c r="H32" s="141">
+      <c r="H32" s="144">
         <f>F32*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I32" s="141">
+      <c r="I32" s="144">
         <f>I27+H32</f>
         <v>889.2</v>
       </c>
       <c r="J32" s="103"/>
       <c r="K32" s="103"/>
-      <c r="L32" s="123" t="s">
-        <v>88</v>
-      </c>
+      <c r="L32" s="123"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="139"/>
+      <c r="A33" s="142"/>
       <c r="B33" s="101" t="s">
         <v>84</v>
       </c>
@@ -6511,15 +6513,15 @@
       <c r="E33" s="102">
         <v>76</v>
       </c>
-      <c r="F33" s="140"/>
-      <c r="G33" s="140"/>
-      <c r="H33" s="141"/>
-      <c r="I33" s="141"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145"/>
+      <c r="H33" s="144"/>
+      <c r="I33" s="144"/>
       <c r="J33" s="103"/>
       <c r="K33" s="103"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="139"/>
+      <c r="A34" s="142"/>
       <c r="B34" s="101" t="s">
         <v>85</v>
       </c>
@@ -6534,15 +6536,15 @@
       <c r="E34" s="102">
         <v>76</v>
       </c>
-      <c r="F34" s="140"/>
-      <c r="G34" s="140"/>
-      <c r="H34" s="141"/>
-      <c r="I34" s="141"/>
+      <c r="F34" s="145"/>
+      <c r="G34" s="145"/>
+      <c r="H34" s="144"/>
+      <c r="I34" s="144"/>
       <c r="J34" s="103"/>
       <c r="K34" s="103"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="139"/>
+      <c r="A35" s="142"/>
       <c r="B35" s="101" t="s">
         <v>86</v>
       </c>
@@ -6557,15 +6559,15 @@
       <c r="E35" s="102">
         <v>76</v>
       </c>
-      <c r="F35" s="140"/>
-      <c r="G35" s="140"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="141"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="145"/>
+      <c r="H35" s="144"/>
+      <c r="I35" s="144"/>
       <c r="J35" s="103"/>
       <c r="K35" s="103"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="139"/>
+      <c r="A36" s="142"/>
       <c r="B36" s="101" t="s">
         <v>87</v>
       </c>
@@ -6580,15 +6582,15 @@
       <c r="E36" s="102">
         <v>76</v>
       </c>
-      <c r="F36" s="140"/>
-      <c r="G36" s="140"/>
-      <c r="H36" s="141"/>
-      <c r="I36" s="141"/>
+      <c r="F36" s="145"/>
+      <c r="G36" s="145"/>
+      <c r="H36" s="144"/>
+      <c r="I36" s="144"/>
       <c r="J36" s="103"/>
       <c r="K36" s="103"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="142">
+      <c r="A37" s="139">
         <f>A32+7</f>
         <v>43734</v>
       </c>
@@ -6606,19 +6608,19 @@
       <c r="E37" s="98">
         <v>76</v>
       </c>
-      <c r="F37" s="143">
+      <c r="F37" s="140">
         <f>SUM(E37:E41)</f>
         <v>380</v>
       </c>
-      <c r="G37" s="143">
+      <c r="G37" s="140">
         <f>G32+F37</f>
         <v>2356</v>
       </c>
-      <c r="H37" s="144">
+      <c r="H37" s="141">
         <f>F37*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I37" s="144">
+      <c r="I37" s="141">
         <f>I32+H37</f>
         <v>1060.2</v>
       </c>
@@ -6626,7 +6628,7 @@
       <c r="K37" s="100"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="142"/>
+      <c r="A38" s="139"/>
       <c r="B38" s="99" t="s">
         <v>84</v>
       </c>
@@ -6641,15 +6643,15 @@
       <c r="E38" s="98">
         <v>76</v>
       </c>
-      <c r="F38" s="143"/>
-      <c r="G38" s="143"/>
-      <c r="H38" s="144"/>
-      <c r="I38" s="144"/>
+      <c r="F38" s="140"/>
+      <c r="G38" s="140"/>
+      <c r="H38" s="141"/>
+      <c r="I38" s="141"/>
       <c r="J38" s="100"/>
       <c r="K38" s="100"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="142"/>
+      <c r="A39" s="139"/>
       <c r="B39" s="99" t="s">
         <v>85</v>
       </c>
@@ -6664,15 +6666,15 @@
       <c r="E39" s="98">
         <v>76</v>
       </c>
-      <c r="F39" s="143"/>
-      <c r="G39" s="143"/>
-      <c r="H39" s="144"/>
-      <c r="I39" s="144"/>
+      <c r="F39" s="140"/>
+      <c r="G39" s="140"/>
+      <c r="H39" s="141"/>
+      <c r="I39" s="141"/>
       <c r="J39" s="100"/>
       <c r="K39" s="100"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="142"/>
+      <c r="A40" s="139"/>
       <c r="B40" s="99" t="s">
         <v>86</v>
       </c>
@@ -6687,15 +6689,15 @@
       <c r="E40" s="98">
         <v>76</v>
       </c>
-      <c r="F40" s="143"/>
-      <c r="G40" s="143"/>
-      <c r="H40" s="144"/>
-      <c r="I40" s="144"/>
+      <c r="F40" s="140"/>
+      <c r="G40" s="140"/>
+      <c r="H40" s="141"/>
+      <c r="I40" s="141"/>
       <c r="J40" s="100"/>
       <c r="K40" s="100"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="142"/>
+      <c r="A41" s="139"/>
       <c r="B41" s="99" t="s">
         <v>87</v>
       </c>
@@ -6710,15 +6712,15 @@
       <c r="E41" s="98">
         <v>76</v>
       </c>
-      <c r="F41" s="143"/>
-      <c r="G41" s="143"/>
-      <c r="H41" s="144"/>
-      <c r="I41" s="144"/>
+      <c r="F41" s="140"/>
+      <c r="G41" s="140"/>
+      <c r="H41" s="141"/>
+      <c r="I41" s="141"/>
       <c r="J41" s="100"/>
       <c r="K41" s="100"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="139">
+      <c r="A42" s="142">
         <f>A37+7</f>
         <v>43741</v>
       </c>
@@ -6736,19 +6738,19 @@
       <c r="E42" s="102">
         <v>76</v>
       </c>
-      <c r="F42" s="140">
+      <c r="F42" s="145">
         <f>SUM(E42:E46)</f>
         <v>304</v>
       </c>
-      <c r="G42" s="140">
+      <c r="G42" s="145">
         <f>G37+F42</f>
         <v>2660</v>
       </c>
-      <c r="H42" s="141">
+      <c r="H42" s="144">
         <f>F42*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I42" s="141">
+      <c r="I42" s="144">
         <f>I37+H42</f>
         <v>1197</v>
       </c>
@@ -6756,7 +6758,7 @@
       <c r="K42" s="103"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="139"/>
+      <c r="A43" s="142"/>
       <c r="B43" s="101" t="s">
         <v>84</v>
       </c>
@@ -6771,15 +6773,15 @@
       <c r="E43" s="102">
         <v>76</v>
       </c>
-      <c r="F43" s="140"/>
-      <c r="G43" s="140"/>
-      <c r="H43" s="141"/>
-      <c r="I43" s="141"/>
+      <c r="F43" s="145"/>
+      <c r="G43" s="145"/>
+      <c r="H43" s="144"/>
+      <c r="I43" s="144"/>
       <c r="J43" s="103"/>
       <c r="K43" s="103"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="139"/>
+      <c r="A44" s="142"/>
       <c r="B44" s="101" t="s">
         <v>85</v>
       </c>
@@ -6794,15 +6796,15 @@
       <c r="E44" s="102">
         <v>76</v>
       </c>
-      <c r="F44" s="140"/>
-      <c r="G44" s="140"/>
-      <c r="H44" s="141"/>
-      <c r="I44" s="141"/>
+      <c r="F44" s="145"/>
+      <c r="G44" s="145"/>
+      <c r="H44" s="144"/>
+      <c r="I44" s="144"/>
       <c r="J44" s="103"/>
       <c r="K44" s="103"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="139"/>
+      <c r="A45" s="142"/>
       <c r="B45" s="101" t="s">
         <v>86</v>
       </c>
@@ -6817,15 +6819,15 @@
       <c r="E45" s="102">
         <v>76</v>
       </c>
-      <c r="F45" s="140"/>
-      <c r="G45" s="140"/>
-      <c r="H45" s="141"/>
-      <c r="I45" s="141"/>
+      <c r="F45" s="145"/>
+      <c r="G45" s="145"/>
+      <c r="H45" s="144"/>
+      <c r="I45" s="144"/>
       <c r="J45" s="103"/>
       <c r="K45" s="103"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="139"/>
+      <c r="A46" s="142"/>
       <c r="B46" s="101" t="s">
         <v>87</v>
       </c>
@@ -6834,18 +6836,16 @@
       <c r="E46" s="102">
         <v>0</v>
       </c>
-      <c r="F46" s="140"/>
-      <c r="G46" s="140"/>
-      <c r="H46" s="141"/>
-      <c r="I46" s="141"/>
+      <c r="F46" s="145"/>
+      <c r="G46" s="145"/>
+      <c r="H46" s="144"/>
+      <c r="I46" s="144"/>
       <c r="J46" s="103"/>
       <c r="K46" s="103"/>
-      <c r="L46" s="123" t="s">
-        <v>89</v>
-      </c>
+      <c r="L46" s="123"/>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="142">
+      <c r="A47" s="139">
         <f>A42+7</f>
         <v>43748</v>
       </c>
@@ -6857,30 +6857,28 @@
       <c r="E47" s="98">
         <v>0</v>
       </c>
-      <c r="F47" s="143">
+      <c r="F47" s="140">
         <f>SUM(E47:E51)</f>
         <v>304</v>
       </c>
-      <c r="G47" s="143">
+      <c r="G47" s="140">
         <f>G42+F47</f>
         <v>2964</v>
       </c>
-      <c r="H47" s="144">
+      <c r="H47" s="141">
         <f>F47*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I47" s="144">
+      <c r="I47" s="141">
         <f>I42+H47</f>
         <v>1333.8</v>
       </c>
       <c r="J47" s="100"/>
       <c r="K47" s="100"/>
-      <c r="L47" s="123" t="s">
-        <v>89</v>
-      </c>
+      <c r="L47" s="123"/>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="142"/>
+      <c r="A48" s="139"/>
       <c r="B48" s="99" t="s">
         <v>84</v>
       </c>
@@ -6895,15 +6893,15 @@
       <c r="E48" s="98">
         <v>76</v>
       </c>
-      <c r="F48" s="143"/>
-      <c r="G48" s="143"/>
-      <c r="H48" s="144"/>
-      <c r="I48" s="144"/>
+      <c r="F48" s="140"/>
+      <c r="G48" s="140"/>
+      <c r="H48" s="141"/>
+      <c r="I48" s="141"/>
       <c r="J48" s="100"/>
       <c r="K48" s="100"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="142"/>
+      <c r="A49" s="139"/>
       <c r="B49" s="99" t="s">
         <v>85</v>
       </c>
@@ -6918,15 +6916,15 @@
       <c r="E49" s="98">
         <v>76</v>
       </c>
-      <c r="F49" s="143"/>
-      <c r="G49" s="143"/>
-      <c r="H49" s="144"/>
-      <c r="I49" s="144"/>
+      <c r="F49" s="140"/>
+      <c r="G49" s="140"/>
+      <c r="H49" s="141"/>
+      <c r="I49" s="141"/>
       <c r="J49" s="100"/>
       <c r="K49" s="100"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="142"/>
+      <c r="A50" s="139"/>
       <c r="B50" s="99" t="s">
         <v>86</v>
       </c>
@@ -6941,15 +6939,15 @@
       <c r="E50" s="98">
         <v>76</v>
       </c>
-      <c r="F50" s="143"/>
-      <c r="G50" s="143"/>
-      <c r="H50" s="144"/>
-      <c r="I50" s="144"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="140"/>
+      <c r="H50" s="141"/>
+      <c r="I50" s="141"/>
       <c r="J50" s="100"/>
       <c r="K50" s="100"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="142"/>
+      <c r="A51" s="139"/>
       <c r="B51" s="99" t="s">
         <v>87</v>
       </c>
@@ -6964,32 +6962,32 @@
       <c r="E51" s="98">
         <v>76</v>
       </c>
-      <c r="F51" s="143"/>
-      <c r="G51" s="143"/>
-      <c r="H51" s="144"/>
-      <c r="I51" s="144"/>
+      <c r="F51" s="140"/>
+      <c r="G51" s="140"/>
+      <c r="H51" s="141"/>
+      <c r="I51" s="141"/>
       <c r="J51" s="100"/>
       <c r="K51" s="100"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="139"/>
+      <c r="A52" s="142"/>
       <c r="B52" s="101"/>
       <c r="C52" s="102"/>
       <c r="D52" s="102"/>
       <c r="E52" s="102"/>
-      <c r="F52" s="140">
+      <c r="F52" s="145">
         <f>SUM(E52:E56)</f>
         <v>0</v>
       </c>
-      <c r="G52" s="140">
+      <c r="G52" s="145">
         <f>G47+F52</f>
         <v>2964</v>
       </c>
-      <c r="H52" s="141">
+      <c r="H52" s="144">
         <f>F52*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I52" s="141">
+      <c r="I52" s="144">
         <f>I47+H52</f>
         <v>1333.8</v>
       </c>
@@ -6997,76 +6995,76 @@
       <c r="K52" s="103"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="139"/>
+      <c r="A53" s="142"/>
       <c r="B53" s="101"/>
       <c r="C53" s="102"/>
       <c r="D53" s="102"/>
       <c r="E53" s="102"/>
-      <c r="F53" s="140"/>
-      <c r="G53" s="140"/>
-      <c r="H53" s="141"/>
-      <c r="I53" s="141"/>
+      <c r="F53" s="145"/>
+      <c r="G53" s="145"/>
+      <c r="H53" s="144"/>
+      <c r="I53" s="144"/>
       <c r="J53" s="103"/>
       <c r="K53" s="103"/>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="139"/>
+      <c r="A54" s="142"/>
       <c r="B54" s="101"/>
       <c r="C54" s="102"/>
       <c r="D54" s="102"/>
       <c r="E54" s="102"/>
-      <c r="F54" s="140"/>
-      <c r="G54" s="140"/>
-      <c r="H54" s="141"/>
-      <c r="I54" s="141"/>
+      <c r="F54" s="145"/>
+      <c r="G54" s="145"/>
+      <c r="H54" s="144"/>
+      <c r="I54" s="144"/>
       <c r="J54" s="103"/>
       <c r="K54" s="103"/>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="139"/>
+      <c r="A55" s="142"/>
       <c r="B55" s="101"/>
       <c r="C55" s="102"/>
       <c r="D55" s="102"/>
       <c r="E55" s="102"/>
-      <c r="F55" s="140"/>
-      <c r="G55" s="140"/>
-      <c r="H55" s="141"/>
-      <c r="I55" s="141"/>
+      <c r="F55" s="145"/>
+      <c r="G55" s="145"/>
+      <c r="H55" s="144"/>
+      <c r="I55" s="144"/>
       <c r="J55" s="103"/>
       <c r="K55" s="103"/>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="139"/>
+      <c r="A56" s="142"/>
       <c r="B56" s="101"/>
       <c r="C56" s="102"/>
       <c r="D56" s="102"/>
       <c r="E56" s="102"/>
-      <c r="F56" s="140"/>
-      <c r="G56" s="140"/>
-      <c r="H56" s="141"/>
-      <c r="I56" s="141"/>
+      <c r="F56" s="145"/>
+      <c r="G56" s="145"/>
+      <c r="H56" s="144"/>
+      <c r="I56" s="144"/>
       <c r="J56" s="103"/>
       <c r="K56" s="103"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="142"/>
+      <c r="A57" s="139"/>
       <c r="B57" s="99"/>
       <c r="C57" s="98"/>
       <c r="D57" s="98"/>
       <c r="E57" s="98"/>
-      <c r="F57" s="143">
+      <c r="F57" s="140">
         <f>SUM(E57:E61)</f>
         <v>0</v>
       </c>
-      <c r="G57" s="143">
+      <c r="G57" s="140">
         <f>G52+F57</f>
         <v>2964</v>
       </c>
-      <c r="H57" s="144">
+      <c r="H57" s="141">
         <f>F57*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I57" s="144">
+      <c r="I57" s="141">
         <f>I52+H57</f>
         <v>1333.8</v>
       </c>
@@ -7074,76 +7072,76 @@
       <c r="K57" s="100"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="142"/>
+      <c r="A58" s="139"/>
       <c r="B58" s="99"/>
       <c r="C58" s="98"/>
       <c r="D58" s="98"/>
       <c r="E58" s="98"/>
-      <c r="F58" s="143"/>
-      <c r="G58" s="143"/>
-      <c r="H58" s="144"/>
-      <c r="I58" s="144"/>
+      <c r="F58" s="140"/>
+      <c r="G58" s="140"/>
+      <c r="H58" s="141"/>
+      <c r="I58" s="141"/>
       <c r="J58" s="100"/>
       <c r="K58" s="100"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="142"/>
+      <c r="A59" s="139"/>
       <c r="B59" s="99"/>
       <c r="C59" s="98"/>
       <c r="D59" s="98"/>
       <c r="E59" s="98"/>
-      <c r="F59" s="143"/>
-      <c r="G59" s="143"/>
-      <c r="H59" s="144"/>
-      <c r="I59" s="144"/>
+      <c r="F59" s="140"/>
+      <c r="G59" s="140"/>
+      <c r="H59" s="141"/>
+      <c r="I59" s="141"/>
       <c r="J59" s="100"/>
       <c r="K59" s="100"/>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="142"/>
+      <c r="A60" s="139"/>
       <c r="B60" s="99"/>
       <c r="C60" s="98"/>
       <c r="D60" s="98"/>
       <c r="E60" s="98"/>
-      <c r="F60" s="143"/>
-      <c r="G60" s="143"/>
-      <c r="H60" s="144"/>
-      <c r="I60" s="144"/>
+      <c r="F60" s="140"/>
+      <c r="G60" s="140"/>
+      <c r="H60" s="141"/>
+      <c r="I60" s="141"/>
       <c r="J60" s="100"/>
       <c r="K60" s="100"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="142"/>
+      <c r="A61" s="139"/>
       <c r="B61" s="99"/>
       <c r="C61" s="98"/>
       <c r="D61" s="98"/>
       <c r="E61" s="98"/>
-      <c r="F61" s="143"/>
-      <c r="G61" s="143"/>
-      <c r="H61" s="144"/>
-      <c r="I61" s="144"/>
+      <c r="F61" s="140"/>
+      <c r="G61" s="140"/>
+      <c r="H61" s="141"/>
+      <c r="I61" s="141"/>
       <c r="J61" s="100"/>
       <c r="K61" s="100"/>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="139"/>
+      <c r="A62" s="142"/>
       <c r="B62" s="101"/>
       <c r="C62" s="102"/>
       <c r="D62" s="102"/>
       <c r="E62" s="102"/>
-      <c r="F62" s="140">
+      <c r="F62" s="145">
         <f>SUM(E62:E66)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="140">
+      <c r="G62" s="145">
         <f>G57+F62</f>
         <v>2964</v>
       </c>
-      <c r="H62" s="141">
+      <c r="H62" s="144">
         <f>F62*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I62" s="141">
+      <c r="I62" s="144">
         <f>I57+H62</f>
         <v>1333.8</v>
       </c>
@@ -7151,120 +7149,120 @@
       <c r="K62" s="103"/>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="139"/>
+      <c r="A63" s="142"/>
       <c r="B63" s="101"/>
       <c r="C63" s="102"/>
       <c r="D63" s="102"/>
       <c r="E63" s="102"/>
-      <c r="F63" s="140"/>
-      <c r="G63" s="140"/>
-      <c r="H63" s="141"/>
-      <c r="I63" s="141"/>
+      <c r="F63" s="145"/>
+      <c r="G63" s="145"/>
+      <c r="H63" s="144"/>
+      <c r="I63" s="144"/>
       <c r="J63" s="103"/>
       <c r="K63" s="103"/>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="139"/>
+      <c r="A64" s="142"/>
       <c r="B64" s="101"/>
       <c r="C64" s="102"/>
       <c r="D64" s="102"/>
       <c r="E64" s="102"/>
-      <c r="F64" s="140"/>
-      <c r="G64" s="140"/>
-      <c r="H64" s="141"/>
-      <c r="I64" s="141"/>
+      <c r="F64" s="145"/>
+      <c r="G64" s="145"/>
+      <c r="H64" s="144"/>
+      <c r="I64" s="144"/>
       <c r="J64" s="103"/>
       <c r="K64" s="103"/>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="139"/>
+      <c r="A65" s="142"/>
       <c r="B65" s="101"/>
       <c r="C65" s="102"/>
       <c r="D65" s="102"/>
       <c r="E65" s="102"/>
-      <c r="F65" s="140"/>
-      <c r="G65" s="140"/>
-      <c r="H65" s="141"/>
-      <c r="I65" s="141"/>
+      <c r="F65" s="145"/>
+      <c r="G65" s="145"/>
+      <c r="H65" s="144"/>
+      <c r="I65" s="144"/>
       <c r="J65" s="103"/>
       <c r="K65" s="103"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="139"/>
+      <c r="A66" s="142"/>
       <c r="B66" s="101"/>
       <c r="C66" s="102"/>
       <c r="D66" s="102"/>
       <c r="E66" s="102"/>
-      <c r="F66" s="140"/>
-      <c r="G66" s="140"/>
-      <c r="H66" s="141"/>
-      <c r="I66" s="141"/>
+      <c r="F66" s="145"/>
+      <c r="G66" s="145"/>
+      <c r="H66" s="144"/>
+      <c r="I66" s="144"/>
       <c r="J66" s="103"/>
       <c r="K66" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="G27:G31"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="G22:G26"/>
-    <mergeCell ref="H22:H26"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="F32:F36"/>
-    <mergeCell ref="G32:G36"/>
-    <mergeCell ref="H32:H36"/>
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="F17:F21"/>
-    <mergeCell ref="G17:G21"/>
-    <mergeCell ref="H17:H21"/>
-    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="F62:F66"/>
+    <mergeCell ref="G62:G66"/>
+    <mergeCell ref="H62:H66"/>
+    <mergeCell ref="I62:I66"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="F52:F56"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="H52:H56"/>
+    <mergeCell ref="I52:I56"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="F57:F61"/>
+    <mergeCell ref="G57:G61"/>
+    <mergeCell ref="H57:H61"/>
+    <mergeCell ref="I57:I61"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="F37:F41"/>
+    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="H37:H41"/>
+    <mergeCell ref="I37:I41"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="F47:F51"/>
+    <mergeCell ref="G47:G51"/>
+    <mergeCell ref="H47:H51"/>
+    <mergeCell ref="I47:I51"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="F42:F46"/>
+    <mergeCell ref="G42:G46"/>
+    <mergeCell ref="H42:H46"/>
+    <mergeCell ref="I42:I46"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="H7:H11"/>
     <mergeCell ref="I7:I11"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="F12:F16"/>
     <mergeCell ref="G12:G16"/>
     <mergeCell ref="H12:H16"/>
     <mergeCell ref="I12:I16"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="F42:F46"/>
-    <mergeCell ref="G42:G46"/>
-    <mergeCell ref="H42:H46"/>
-    <mergeCell ref="I42:I46"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="F47:F51"/>
-    <mergeCell ref="G47:G51"/>
-    <mergeCell ref="H47:H51"/>
-    <mergeCell ref="I47:I51"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="F37:F41"/>
-    <mergeCell ref="G37:G41"/>
-    <mergeCell ref="H37:H41"/>
-    <mergeCell ref="I37:I41"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="F57:F61"/>
-    <mergeCell ref="G57:G61"/>
-    <mergeCell ref="H57:H61"/>
-    <mergeCell ref="I57:I61"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="F52:F56"/>
-    <mergeCell ref="G52:G56"/>
-    <mergeCell ref="H52:H56"/>
-    <mergeCell ref="I52:I56"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="F62:F66"/>
-    <mergeCell ref="G62:G66"/>
-    <mergeCell ref="H62:H66"/>
-    <mergeCell ref="I62:I66"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="G32:G36"/>
+    <mergeCell ref="H32:H36"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="G22:G26"/>
+    <mergeCell ref="H22:H26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="G27:G31"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="I27:I31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="portrait"/>

</xml_diff>